<commit_message>
Added population concentration data
</commit_message>
<xml_diff>
--- a/Data/Vinmonopolet/B&R_data.xlsx
+++ b/Data/Vinmonopolet/B&R_data.xlsx
@@ -420,7 +420,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Monthly_salary</t>
+          <t>prop_spread</t>
         </is>
       </c>
     </row>
@@ -468,7 +468,7 @@
         <v>6718960</v>
       </c>
       <c r="M2">
-        <v>65900</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="3">
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>57360</v>
+        <v>16.57</v>
       </c>
     </row>
     <row r="4">
@@ -562,7 +562,7 @@
         <v>1160696</v>
       </c>
       <c r="M4">
-        <v>68170</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -609,7 +609,7 @@
         <v>254352</v>
       </c>
       <c r="M5">
-        <v>59760</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="6">
@@ -656,7 +656,7 @@
         <v>234743</v>
       </c>
       <c r="M6">
-        <v>62030</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="7">
@@ -703,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>55420</v>
+        <v>28.17</v>
       </c>
     </row>
     <row r="8">
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>52850</v>
+        <v>37.72</v>
       </c>
     </row>
     <row r="9">
@@ -797,7 +797,7 @@
         <v>6540</v>
       </c>
       <c r="M9">
-        <v>55250</v>
+        <v>45.64</v>
       </c>
     </row>
     <row r="10">
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="M10">
-        <v>54250</v>
+        <v>19.32</v>
       </c>
     </row>
     <row r="11">
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>57680</v>
+        <v>17.26</v>
       </c>
     </row>
     <row r="12">
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <v>59110</v>
+        <v>11.19</v>
       </c>
     </row>
     <row r="13">
@@ -985,7 +985,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>56490</v>
+        <v>9.93</v>
       </c>
     </row>
     <row r="14">
@@ -1032,7 +1032,7 @@
         <v>232445</v>
       </c>
       <c r="M14">
-        <v>67920</v>
+        <v>9.359999999999999</v>
       </c>
     </row>
     <row r="15">
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>63280</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="16">
@@ -1126,7 +1126,7 @@
         <v>97415</v>
       </c>
       <c r="M16">
-        <v>58520</v>
+        <v>18.04</v>
       </c>
     </row>
     <row r="17">
@@ -1173,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>55800</v>
+        <v>76.69</v>
       </c>
     </row>
     <row r="18">
@@ -1220,7 +1220,7 @@
         <v>51366</v>
       </c>
       <c r="M18">
-        <v>54500</v>
+        <v>68.68000000000001</v>
       </c>
     </row>
     <row r="19">
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>56550</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="20">
@@ -1314,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>59460</v>
+        <v>26.84</v>
       </c>
     </row>
     <row r="21">
@@ -1361,7 +1361,7 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>59670</v>
+        <v>43.26</v>
       </c>
     </row>
     <row r="22">
@@ -1408,7 +1408,7 @@
         <v>27668</v>
       </c>
       <c r="M22">
-        <v>58920</v>
+        <v>37.08</v>
       </c>
     </row>
     <row r="23">
@@ -1455,7 +1455,7 @@
         <v>12914</v>
       </c>
       <c r="M23">
-        <v>58220</v>
+        <v>11.44</v>
       </c>
     </row>
     <row r="24">
@@ -1502,7 +1502,7 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <v>63170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25">
@@ -1549,7 +1549,7 @@
         <v>19798</v>
       </c>
       <c r="M25">
-        <v>55890</v>
+        <v>54.75</v>
       </c>
     </row>
     <row r="26">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D26">
@@ -1589,14 +1589,11 @@
       <c r="J26">
         <v>0.2423966295353834</v>
       </c>
-      <c r="K26">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L26">
         <v>158591</v>
       </c>
       <c r="M26">
-        <v>57120</v>
+        <v>8.640000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -1612,7 +1609,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D27">
@@ -1636,14 +1633,11 @@
       <c r="J27">
         <v>1.22065478644859</v>
       </c>
-      <c r="K27">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L27">
         <v>225946</v>
       </c>
       <c r="M27">
-        <v>57800</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="28">
@@ -1659,7 +1653,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D28">
@@ -1683,14 +1677,11 @@
       <c r="J28">
         <v>0.02974320608000384</v>
       </c>
-      <c r="K28">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L28">
         <v>421789</v>
       </c>
       <c r="M28">
-        <v>58100</v>
+        <v>6.97</v>
       </c>
     </row>
     <row r="29">
@@ -1706,7 +1697,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D29">
@@ -1730,14 +1721,11 @@
       <c r="J29">
         <v>0.1095759996931654</v>
       </c>
-      <c r="K29">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
-        <v>56310</v>
+        <v>83.94</v>
       </c>
     </row>
     <row r="30">
@@ -1753,7 +1741,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D30">
@@ -1784,7 +1772,7 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>55350</v>
+        <v>52.05</v>
       </c>
     </row>
     <row r="31">
@@ -1800,7 +1788,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D31">
@@ -1824,14 +1812,11 @@
       <c r="J31">
         <v>0.1310903619924779</v>
       </c>
-      <c r="K31">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L31">
         <v>27968</v>
       </c>
       <c r="M31">
-        <v>57490</v>
+        <v>32.33</v>
       </c>
     </row>
     <row r="32">
@@ -1847,7 +1832,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D32">
@@ -1871,14 +1856,11 @@
       <c r="J32">
         <v>0.2212560507591561</v>
       </c>
-      <c r="K32">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
-        <v>59950</v>
+        <v>16.31</v>
       </c>
     </row>
     <row r="33">
@@ -1894,7 +1876,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D33">
@@ -1925,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>55420</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="34">
@@ -1941,7 +1923,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D34">
@@ -1965,14 +1947,11 @@
       <c r="J34">
         <v>0.332077970727406</v>
       </c>
-      <c r="K34">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L34">
         <v>60697</v>
       </c>
       <c r="M34">
-        <v>54120</v>
+        <v>26.83</v>
       </c>
     </row>
     <row r="35">
@@ -1988,7 +1967,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D35">
@@ -2012,14 +1991,11 @@
       <c r="J35">
         <v>0.04812428799808574</v>
       </c>
-      <c r="K35">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L35">
         <v>253196</v>
       </c>
       <c r="M35">
-        <v>51840</v>
+        <v>35.33</v>
       </c>
     </row>
     <row r="36">
@@ -2035,7 +2011,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D36">
@@ -2059,14 +2035,11 @@
       <c r="J36">
         <v>0.3492938422089224</v>
       </c>
-      <c r="K36">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
-        <v>53650</v>
+        <v>24.88</v>
       </c>
     </row>
     <row r="37">
@@ -2082,7 +2055,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D37">
@@ -2106,14 +2079,11 @@
       <c r="J37">
         <v>0.120554396058822</v>
       </c>
-      <c r="K37">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
-        <v>55580</v>
+        <v>6.03</v>
       </c>
     </row>
     <row r="38">
@@ -2129,7 +2099,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D38">
@@ -2160,7 +2130,7 @@
         <v>15583</v>
       </c>
       <c r="M38">
-        <v>57240</v>
+        <v>17.16</v>
       </c>
     </row>
     <row r="39">
@@ -2176,7 +2146,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D39">
@@ -2200,14 +2170,11 @@
       <c r="J39">
         <v>0.2994430281898573</v>
       </c>
-      <c r="K39">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L39">
         <v>15484</v>
       </c>
       <c r="M39">
-        <v>54160</v>
+        <v>37.19</v>
       </c>
     </row>
     <row r="40">
@@ -2223,7 +2190,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D40">
@@ -2247,14 +2214,11 @@
       <c r="J40">
         <v>0.1242853402984652</v>
       </c>
-      <c r="K40">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L40">
         <v>105592</v>
       </c>
       <c r="M40">
-        <v>53830</v>
+        <v>34.62</v>
       </c>
     </row>
     <row r="41">
@@ -2270,7 +2234,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D41">
@@ -2301,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="M41">
-        <v>55790</v>
+        <v>52.23</v>
       </c>
     </row>
     <row r="42">
@@ -2317,7 +2281,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D42">
@@ -2341,14 +2305,11 @@
       <c r="J42">
         <v>0.130676384825917</v>
       </c>
-      <c r="K42">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
-        <v>57720</v>
+        <v>71.59999999999999</v>
       </c>
     </row>
     <row r="43">
@@ -2364,7 +2325,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D43">
@@ -2395,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="M43">
-        <v>53590</v>
+        <v>76.41</v>
       </c>
     </row>
     <row r="44">
@@ -2411,7 +2372,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D44">
@@ -2442,7 +2403,7 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>53780</v>
+        <v>65.77</v>
       </c>
     </row>
     <row r="45">
@@ -2458,7 +2419,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D45">
@@ -2482,14 +2443,11 @@
       <c r="J45">
         <v>0.9417159190798167</v>
       </c>
-      <c r="K45">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L45">
         <v>29985</v>
       </c>
       <c r="M45">
-        <v>58000</v>
+        <v>32.02</v>
       </c>
     </row>
     <row r="46">
@@ -2505,7 +2463,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D46">
@@ -2529,14 +2487,11 @@
       <c r="J46">
         <v>0.1746207155434114</v>
       </c>
-      <c r="K46">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L46">
         <v>20085</v>
       </c>
       <c r="M46">
-        <v>53570</v>
+        <v>51.76</v>
       </c>
     </row>
     <row r="47">
@@ -2552,7 +2507,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D47">
@@ -2576,14 +2531,11 @@
       <c r="J47">
         <v>0.1342763104211891</v>
       </c>
-      <c r="K47">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L47">
         <v>20798</v>
       </c>
       <c r="M47">
-        <v>54860</v>
+        <v>99.95</v>
       </c>
     </row>
     <row r="48">
@@ -2599,7 +2551,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D48">
@@ -2630,7 +2582,7 @@
         <v>0</v>
       </c>
       <c r="M48">
-        <v>57710</v>
+        <v>81.22</v>
       </c>
     </row>
     <row r="49">
@@ -2646,7 +2598,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D49">
@@ -2670,14 +2622,11 @@
       <c r="J49">
         <v>0.3636450666718419</v>
       </c>
-      <c r="K49">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L49">
         <v>13654</v>
       </c>
       <c r="M49">
-        <v>55450</v>
+        <v>26.78</v>
       </c>
     </row>
     <row r="50">
@@ -2693,7 +2642,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MC8re og Romsdal</t>
         </is>
       </c>
       <c r="D50">
@@ -2724,7 +2673,7 @@
         <v>102285</v>
       </c>
       <c r="M50">
-        <v>51530</v>
+        <v>76.48</v>
       </c>
     </row>
     <row r="51">
@@ -2740,7 +2689,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D51">
@@ -2764,14 +2713,11 @@
       <c r="J51">
         <v>0.3665115095323905</v>
       </c>
-      <c r="K51">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L51">
         <v>53918</v>
       </c>
       <c r="M51">
-        <v>54120</v>
+        <v>47.24</v>
       </c>
     </row>
     <row r="52">
@@ -2787,7 +2733,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>MØRE OG ROMSDAL</t>
         </is>
       </c>
       <c r="D52">
@@ -2811,14 +2757,11 @@
       <c r="J52">
         <v>0.1626791499749644</v>
       </c>
-      <c r="K52">
-        <v>8.921212499999999</v>
-      </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52">
-        <v>54770</v>
+        <v>33.09</v>
       </c>
     </row>
     <row r="53">
@@ -2865,7 +2808,7 @@
         <v>581309</v>
       </c>
       <c r="M53">
-        <v>58440</v>
+        <v>8.050000000000001</v>
       </c>
     </row>
     <row r="54">
@@ -2912,7 +2855,7 @@
         <v>210944</v>
       </c>
       <c r="M54">
-        <v>55930</v>
+        <v>15.42</v>
       </c>
     </row>
     <row r="55">
@@ -2959,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>52450</v>
+        <v>62.33</v>
       </c>
     </row>
     <row r="56">
@@ -3006,7 +2949,7 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>53310</v>
+        <v>52.02</v>
       </c>
     </row>
     <row r="57">
@@ -3053,7 +2996,7 @@
         <v>30622</v>
       </c>
       <c r="M57">
-        <v>54840</v>
+        <v>27.55</v>
       </c>
     </row>
     <row r="58">
@@ -3100,7 +3043,7 @@
         <v>8237</v>
       </c>
       <c r="M58">
-        <v>53350</v>
+        <v>74.59</v>
       </c>
     </row>
     <row r="59">
@@ -3147,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>54710</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60">
@@ -3194,7 +3137,7 @@
         <v>4405</v>
       </c>
       <c r="M60">
-        <v>54650</v>
+        <v>53.15</v>
       </c>
     </row>
     <row r="61">
@@ -3241,7 +3184,7 @@
         <v>26113</v>
       </c>
       <c r="M61">
-        <v>55170</v>
+        <v>18.31</v>
       </c>
     </row>
     <row r="62">
@@ -3288,7 +3231,7 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>53140</v>
+        <v>67.05</v>
       </c>
     </row>
     <row r="63">
@@ -3335,7 +3278,7 @@
         <v>31160</v>
       </c>
       <c r="M63">
-        <v>54870</v>
+        <v>25.27</v>
       </c>
     </row>
     <row r="64">
@@ -3382,7 +3325,7 @@
         <v>10406</v>
       </c>
       <c r="M64">
-        <v>50170</v>
+        <v>40.57</v>
       </c>
     </row>
     <row r="65">
@@ -3429,7 +3372,7 @@
         <v>0</v>
       </c>
       <c r="M65">
-        <v>49190</v>
+        <v>57.79</v>
       </c>
     </row>
     <row r="66">
@@ -3476,7 +3419,7 @@
         <v>3015</v>
       </c>
       <c r="M66">
-        <v>55160</v>
+        <v>81.08</v>
       </c>
     </row>
     <row r="67">
@@ -3523,7 +3466,7 @@
         <v>0</v>
       </c>
       <c r="M67">
-        <v>53670</v>
+        <v>23.17</v>
       </c>
     </row>
     <row r="68">
@@ -3570,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="M68">
-        <v>53740</v>
+        <v>39.24</v>
       </c>
     </row>
     <row r="69">
@@ -3617,7 +3560,7 @@
         <v>166181</v>
       </c>
       <c r="M69">
-        <v>55660</v>
+        <v>16.6</v>
       </c>
     </row>
     <row r="70">
@@ -3664,7 +3607,7 @@
         <v>0</v>
       </c>
       <c r="M70">
-        <v>57180</v>
+        <v>72.16</v>
       </c>
     </row>
     <row r="71">
@@ -3711,7 +3654,7 @@
         <v>0</v>
       </c>
       <c r="M71">
-        <v>50870</v>
+        <v>12.67</v>
       </c>
     </row>
     <row r="72">
@@ -3758,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="M72">
-        <v>55720</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73">
@@ -3805,7 +3748,7 @@
         <v>33851</v>
       </c>
       <c r="M73">
-        <v>55570</v>
+        <v>42.33</v>
       </c>
     </row>
     <row r="74">
@@ -3852,7 +3795,7 @@
         <v>10679</v>
       </c>
       <c r="M74">
-        <v>53430</v>
+        <v>67.56999999999999</v>
       </c>
     </row>
     <row r="75">
@@ -3899,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="M75">
-        <v>51370</v>
+        <v>99.91</v>
       </c>
     </row>
     <row r="76">
@@ -3946,7 +3889,7 @@
         <v>31832</v>
       </c>
       <c r="M76">
-        <v>54350</v>
+        <v>33.42</v>
       </c>
     </row>
     <row r="77">
@@ -3993,7 +3936,7 @@
         <v>34390</v>
       </c>
       <c r="M77">
-        <v>54740</v>
+        <v>24.69</v>
       </c>
     </row>
     <row r="78">
@@ -4040,7 +3983,7 @@
         <v>0</v>
       </c>
       <c r="M78">
-        <v>53790</v>
+        <v>53.88</v>
       </c>
     </row>
     <row r="79">
@@ -4087,7 +4030,7 @@
         <v>17742</v>
       </c>
       <c r="M79">
-        <v>55810</v>
+        <v>90.83</v>
       </c>
     </row>
     <row r="80">
@@ -4134,7 +4077,7 @@
         <v>0</v>
       </c>
       <c r="M80">
-        <v>52330</v>
+        <v>17.38</v>
       </c>
     </row>
     <row r="81">
@@ -4181,7 +4124,7 @@
         <v>5117</v>
       </c>
       <c r="M81">
-        <v>53360</v>
+        <v>48.57</v>
       </c>
     </row>
     <row r="82">
@@ -4228,7 +4171,7 @@
         <v>0</v>
       </c>
       <c r="M82">
-        <v>50230</v>
+        <v>30.22</v>
       </c>
     </row>
     <row r="83">
@@ -4275,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="M83">
-        <v>50970</v>
+        <v>12.45</v>
       </c>
     </row>
     <row r="84">
@@ -4322,7 +4265,7 @@
         <v>26138</v>
       </c>
       <c r="M84">
-        <v>51570</v>
+        <v>99.84</v>
       </c>
     </row>
     <row r="85">
@@ -4369,7 +4312,7 @@
         <v>92343</v>
       </c>
       <c r="M85">
-        <v>53040</v>
+        <v>36.08</v>
       </c>
     </row>
     <row r="86">
@@ -4416,7 +4359,7 @@
         <v>441299</v>
       </c>
       <c r="M86">
-        <v>52810</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="87">
@@ -4463,7 +4406,7 @@
         <v>55407</v>
       </c>
       <c r="M87">
-        <v>54300</v>
+        <v>24.62</v>
       </c>
     </row>
     <row r="88">
@@ -4510,7 +4453,7 @@
         <v>24161</v>
       </c>
       <c r="M88">
-        <v>52530</v>
+        <v>64.81</v>
       </c>
     </row>
     <row r="89">
@@ -4557,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="M89">
-        <v>52470</v>
+        <v>44.25</v>
       </c>
     </row>
     <row r="90">
@@ -4604,7 +4547,7 @@
         <v>75509</v>
       </c>
       <c r="M90">
-        <v>54470</v>
+        <v>31.37</v>
       </c>
     </row>
     <row r="91">
@@ -4651,7 +4594,7 @@
         <v>94508</v>
       </c>
       <c r="M91">
-        <v>54180</v>
+        <v>35.14</v>
       </c>
     </row>
     <row r="92">
@@ -4698,7 +4641,7 @@
         <v>138321</v>
       </c>
       <c r="M92">
-        <v>48910</v>
+        <v>27.46</v>
       </c>
     </row>
     <row r="93">
@@ -4745,7 +4688,7 @@
         <v>34894</v>
       </c>
       <c r="M93">
-        <v>55490</v>
+        <v>68.05</v>
       </c>
     </row>
     <row r="94">
@@ -4761,7 +4704,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D94">
@@ -4785,14 +4728,11 @@
       <c r="J94">
         <v>0.2442896293388739</v>
       </c>
-      <c r="K94">
-        <v>203.3475</v>
-      </c>
       <c r="L94">
         <v>86004</v>
       </c>
       <c r="M94">
-        <v>55470</v>
+        <v>12.55</v>
       </c>
     </row>
     <row r="95">
@@ -4808,7 +4748,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D95">
@@ -4832,14 +4772,11 @@
       <c r="J95">
         <v>0.4179704058803027</v>
       </c>
-      <c r="K95">
-        <v>203.3475</v>
-      </c>
       <c r="L95">
         <v>57442</v>
       </c>
       <c r="M95">
-        <v>58280</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="96">
@@ -4855,7 +4792,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D96">
@@ -4879,14 +4816,11 @@
       <c r="J96">
         <v>0.363065088781134</v>
       </c>
-      <c r="K96">
-        <v>203.3475</v>
-      </c>
       <c r="L96">
         <v>0</v>
       </c>
       <c r="M96">
-        <v>54260</v>
+        <v>8.789999999999999</v>
       </c>
     </row>
     <row r="97">
@@ -4902,7 +4836,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D97">
@@ -4926,14 +4860,11 @@
       <c r="J97">
         <v>0.7875826270011952</v>
       </c>
-      <c r="K97">
-        <v>203.3475</v>
-      </c>
       <c r="L97">
         <v>47847</v>
       </c>
       <c r="M97">
-        <v>56710</v>
+        <v>6.31</v>
       </c>
     </row>
     <row r="98">
@@ -4949,7 +4880,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D98">
@@ -4973,14 +4904,11 @@
       <c r="J98">
         <v>0.1880250164650877</v>
       </c>
-      <c r="K98">
-        <v>203.3475</v>
-      </c>
       <c r="L98">
         <v>0</v>
       </c>
       <c r="M98">
-        <v>59290</v>
+        <v>37.33</v>
       </c>
     </row>
     <row r="99">
@@ -4996,7 +4924,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>C_x0018_stfold</t>
         </is>
       </c>
       <c r="D99">
@@ -5020,14 +4948,11 @@
       <c r="J99">
         <v>12.8910270925836</v>
       </c>
-      <c r="K99">
-        <v>203.3475</v>
-      </c>
       <c r="L99">
         <v>55235</v>
       </c>
       <c r="M99">
-        <v>55790</v>
+        <v>22.17</v>
       </c>
     </row>
     <row r="100">
@@ -5043,7 +4968,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>C_x0018_stfold</t>
         </is>
       </c>
       <c r="D100">
@@ -5067,14 +4992,11 @@
       <c r="J100">
         <v>10.7889312979334</v>
       </c>
-      <c r="K100">
-        <v>203.3475</v>
-      </c>
       <c r="L100">
         <v>0</v>
       </c>
       <c r="M100">
-        <v>55650</v>
+        <v>30.95</v>
       </c>
     </row>
     <row r="101">
@@ -5090,7 +5012,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>C_x0018_stfold</t>
         </is>
       </c>
       <c r="D101">
@@ -5114,14 +5036,11 @@
       <c r="J101">
         <v>11.51837921725955</v>
       </c>
-      <c r="K101">
-        <v>203.3475</v>
-      </c>
       <c r="L101">
         <v>0</v>
       </c>
       <c r="M101">
-        <v>53250</v>
+        <v>50.19</v>
       </c>
     </row>
     <row r="102">
@@ -5137,7 +5056,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D102">
@@ -5161,14 +5080,11 @@
       <c r="J102">
         <v>0.5653232738183865</v>
       </c>
-      <c r="K102">
-        <v>203.3475</v>
-      </c>
       <c r="L102">
         <v>6053</v>
       </c>
       <c r="M102">
-        <v>53520</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="103">
@@ -5184,7 +5100,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>ØSTFOLD</t>
         </is>
       </c>
       <c r="D103">
@@ -5208,14 +5124,11 @@
       <c r="J103">
         <v>0.2023578968498255</v>
       </c>
-      <c r="K103">
-        <v>203.3475</v>
-      </c>
       <c r="L103">
         <v>0</v>
       </c>
       <c r="M103">
-        <v>52480</v>
+        <v>36.76</v>
       </c>
     </row>
     <row r="104">
@@ -5231,7 +5144,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>C_x0018_stfold</t>
         </is>
       </c>
       <c r="D104">
@@ -5255,14 +5168,11 @@
       <c r="J104">
         <v>18.95264226153718</v>
       </c>
-      <c r="K104">
-        <v>203.3475</v>
-      </c>
       <c r="L104">
         <v>0</v>
       </c>
       <c r="M104">
-        <v>53220</v>
+        <v>49.15</v>
       </c>
     </row>
     <row r="105">
@@ -5278,7 +5188,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Østfold</t>
+          <t>C_x0018_stfold</t>
         </is>
       </c>
       <c r="D105">
@@ -5302,14 +5212,11 @@
       <c r="J105">
         <v>21.04270846108081</v>
       </c>
-      <c r="K105">
-        <v>203.3475</v>
-      </c>
       <c r="L105">
         <v>0</v>
       </c>
       <c r="M105">
-        <v>52180</v>
+        <v>99.93000000000001</v>
       </c>
     </row>
     <row r="106">
@@ -5356,7 +5263,7 @@
         <v>345089</v>
       </c>
       <c r="M106">
-        <v>76170</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="107">
@@ -5403,7 +5310,7 @@
         <v>198740</v>
       </c>
       <c r="M107">
-        <v>69150</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="108">
@@ -5450,7 +5357,7 @@
         <v>269120</v>
       </c>
       <c r="M108">
-        <v>59910</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="109">
@@ -5497,7 +5404,7 @@
         <v>105100</v>
       </c>
       <c r="M109">
-        <v>65160</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="110">
@@ -5544,7 +5451,7 @@
         <v>1188458</v>
       </c>
       <c r="M110">
-        <v>56350</v>
+        <v>7.79</v>
       </c>
     </row>
     <row r="111">
@@ -5591,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="M111">
-        <v>65170</v>
+        <v>9.24</v>
       </c>
     </row>
     <row r="112">
@@ -5638,7 +5545,7 @@
         <v>0</v>
       </c>
       <c r="M112">
-        <v>65260</v>
+        <v>15.16</v>
       </c>
     </row>
     <row r="113">
@@ -5685,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="M113">
-        <v>60460</v>
+        <v>14.79</v>
       </c>
     </row>
     <row r="114">
@@ -5732,7 +5639,7 @@
         <v>0</v>
       </c>
       <c r="M114">
-        <v>60530</v>
+        <v>13.92</v>
       </c>
     </row>
     <row r="115">
@@ -5779,7 +5686,7 @@
         <v>0</v>
       </c>
       <c r="M115">
-        <v>55610</v>
+        <v>19.86</v>
       </c>
     </row>
     <row r="116">
@@ -5826,7 +5733,7 @@
         <v>0</v>
       </c>
       <c r="M116">
-        <v>60400</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="117">
@@ -5873,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="M117">
-        <v>60090</v>
+        <v>2.83</v>
       </c>
     </row>
     <row r="118">
@@ -5920,7 +5827,7 @@
         <v>0</v>
       </c>
       <c r="M118">
-        <v>53650</v>
+        <v>39.24</v>
       </c>
     </row>
     <row r="119">
@@ -5967,7 +5874,7 @@
         <v>14080</v>
       </c>
       <c r="M119">
-        <v>54820</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="120">
@@ -6014,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="M120">
-        <v>61000</v>
+        <v>23.61</v>
       </c>
     </row>
     <row r="121">
@@ -6061,7 +5968,7 @@
         <v>0</v>
       </c>
       <c r="M121">
-        <v>62260</v>
+        <v>5.93</v>
       </c>
     </row>
     <row r="122">
@@ -6108,7 +6015,7 @@
         <v>0</v>
       </c>
       <c r="M122">
-        <v>56180</v>
+        <v>34.99</v>
       </c>
     </row>
     <row r="123">
@@ -6155,7 +6062,7 @@
         <v>0</v>
       </c>
       <c r="M123">
-        <v>53850</v>
+        <v>25.52</v>
       </c>
     </row>
     <row r="124">
@@ -6202,7 +6109,7 @@
         <v>0</v>
       </c>
       <c r="M124">
-        <v>54330</v>
+        <v>20.13</v>
       </c>
     </row>
     <row r="125">
@@ -6249,7 +6156,7 @@
         <v>0</v>
       </c>
       <c r="M125">
-        <v>55310</v>
+        <v>16.97</v>
       </c>
     </row>
     <row r="126">
@@ -6296,7 +6203,7 @@
         <v>0</v>
       </c>
       <c r="M126">
-        <v>54120</v>
+        <v>61.39</v>
       </c>
     </row>
     <row r="127">
@@ -6343,7 +6250,7 @@
         <v>39925</v>
       </c>
       <c r="M127">
-        <v>57890</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="128">
@@ -6390,7 +6297,7 @@
         <v>74917</v>
       </c>
       <c r="M128">
-        <v>61950</v>
+        <v>12.96</v>
       </c>
     </row>
     <row r="129">
@@ -6437,7 +6344,7 @@
         <v>68591</v>
       </c>
       <c r="M129">
-        <v>54350</v>
+        <v>25.94</v>
       </c>
     </row>
     <row r="130">
@@ -6484,7 +6391,7 @@
         <v>42801</v>
       </c>
       <c r="M130">
-        <v>63090</v>
+        <v>34.9</v>
       </c>
     </row>
     <row r="131">
@@ -6531,7 +6438,7 @@
         <v>0</v>
       </c>
       <c r="M131">
-        <v>62170</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="132">
@@ -6578,7 +6485,7 @@
         <v>0</v>
       </c>
       <c r="M132">
-        <v>55870</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="133">
@@ -6625,7 +6532,7 @@
         <v>0</v>
       </c>
       <c r="M133">
-        <v>53460</v>
+        <v>28.21</v>
       </c>
     </row>
     <row r="134">
@@ -6672,7 +6579,7 @@
         <v>0</v>
       </c>
       <c r="M134">
-        <v>52680</v>
+        <v>57.03</v>
       </c>
     </row>
     <row r="135">
@@ -6719,7 +6626,7 @@
         <v>0</v>
       </c>
       <c r="M135">
-        <v>51400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="136">
@@ -6766,7 +6673,7 @@
         <v>11478</v>
       </c>
       <c r="M136">
-        <v>52460</v>
+        <v>35.02</v>
       </c>
     </row>
     <row r="137">
@@ -6813,7 +6720,7 @@
         <v>249121</v>
       </c>
       <c r="M137">
-        <v>51770</v>
+        <v>32.83</v>
       </c>
     </row>
     <row r="138">
@@ -6860,7 +6767,7 @@
         <v>280203</v>
       </c>
       <c r="M138">
-        <v>54330</v>
+        <v>39.27</v>
       </c>
     </row>
     <row r="139">
@@ -6907,7 +6814,7 @@
         <v>46767</v>
       </c>
       <c r="M139">
-        <v>53180</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="140">
@@ -6954,7 +6861,7 @@
         <v>424432</v>
       </c>
       <c r="M140">
-        <v>52120</v>
+        <v>35.88</v>
       </c>
     </row>
     <row r="141">
@@ -7001,7 +6908,7 @@
         <v>16265</v>
       </c>
       <c r="M141">
-        <v>51990</v>
+        <v>85.2</v>
       </c>
     </row>
     <row r="142">
@@ -7048,7 +6955,7 @@
         <v>0</v>
       </c>
       <c r="M142">
-        <v>54310</v>
+        <v>63.61</v>
       </c>
     </row>
     <row r="143">
@@ -7095,7 +7002,7 @@
         <v>0</v>
       </c>
       <c r="M143">
-        <v>50890</v>
+        <v>73.98</v>
       </c>
     </row>
     <row r="144">
@@ -7142,7 +7049,7 @@
         <v>44137</v>
       </c>
       <c r="M144">
-        <v>51010</v>
+        <v>79.69</v>
       </c>
     </row>
     <row r="145">
@@ -7189,7 +7096,7 @@
         <v>28103</v>
       </c>
       <c r="M145">
-        <v>54520</v>
+        <v>25.48</v>
       </c>
     </row>
     <row r="146">
@@ -7236,7 +7143,7 @@
         <v>195164</v>
       </c>
       <c r="M146">
-        <v>59110</v>
+        <v>10.96</v>
       </c>
     </row>
     <row r="147">
@@ -7283,7 +7190,7 @@
         <v>484011</v>
       </c>
       <c r="M147">
-        <v>58200</v>
+        <v>12.71</v>
       </c>
     </row>
     <row r="148">
@@ -7330,7 +7237,7 @@
         <v>152223</v>
       </c>
       <c r="M148">
-        <v>55960</v>
+        <v>21.77</v>
       </c>
     </row>
     <row r="149">
@@ -7377,7 +7284,7 @@
         <v>111736</v>
       </c>
       <c r="M149">
-        <v>53530</v>
+        <v>42.13</v>
       </c>
     </row>
     <row r="150">
@@ -7424,7 +7331,7 @@
         <v>0</v>
       </c>
       <c r="M150">
-        <v>51980</v>
+        <v>40.21</v>
       </c>
     </row>
     <row r="151">
@@ -7471,7 +7378,7 @@
         <v>0</v>
       </c>
       <c r="M151">
-        <v>55300</v>
+        <v>34.86</v>
       </c>
     </row>
     <row r="152">
@@ -7518,7 +7425,7 @@
         <v>0</v>
       </c>
       <c r="M152">
-        <v>51920</v>
+        <v>68.98999999999999</v>
       </c>
     </row>
     <row r="153">
@@ -7565,7 +7472,7 @@
         <v>0</v>
       </c>
       <c r="M153">
-        <v>53430</v>
+        <v>59.52</v>
       </c>
     </row>
     <row r="154">
@@ -7612,7 +7519,7 @@
         <v>0</v>
       </c>
       <c r="M154">
-        <v>51240</v>
+        <v>61.27</v>
       </c>
     </row>
     <row r="155">
@@ -7659,7 +7566,7 @@
         <v>4301</v>
       </c>
       <c r="M155">
-        <v>50940</v>
+        <v>72.93000000000001</v>
       </c>
     </row>
     <row r="156">
@@ -7706,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="M156">
-        <v>51100</v>
+        <v>69.66</v>
       </c>
     </row>
     <row r="157">
@@ -7753,7 +7660,7 @@
         <v>0</v>
       </c>
       <c r="M157">
-        <v>49650</v>
+        <v>62.41</v>
       </c>
     </row>
     <row r="158">
@@ -7800,7 +7707,7 @@
         <v>0</v>
       </c>
       <c r="M158">
-        <v>55300</v>
+        <v>24.76</v>
       </c>
     </row>
     <row r="159">
@@ -7847,7 +7754,7 @@
         <v>62906</v>
       </c>
       <c r="M159">
-        <v>50440</v>
+        <v>55.25</v>
       </c>
     </row>
     <row r="160">
@@ -7894,7 +7801,7 @@
         <v>8870</v>
       </c>
       <c r="M160">
-        <v>55570</v>
+        <v>50.62</v>
       </c>
     </row>
     <row r="161">
@@ -7941,7 +7848,7 @@
         <v>19284</v>
       </c>
       <c r="M161">
-        <v>50260</v>
+        <v>55.54</v>
       </c>
     </row>
     <row r="162">
@@ -7988,7 +7895,7 @@
         <v>0</v>
       </c>
       <c r="M162">
-        <v>49220</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="163">
@@ -8035,7 +7942,7 @@
         <v>44363</v>
       </c>
       <c r="M163">
-        <v>48880</v>
+        <v>77.44</v>
       </c>
     </row>
     <row r="164">
@@ -8082,7 +7989,7 @@
         <v>0</v>
       </c>
       <c r="M164">
-        <v>51730</v>
+        <v>60.85</v>
       </c>
     </row>
     <row r="165">
@@ -8129,7 +8036,7 @@
         <v>0</v>
       </c>
       <c r="M165">
-        <v>51800</v>
+        <v>47.7</v>
       </c>
     </row>
     <row r="166">
@@ -8176,7 +8083,7 @@
         <v>7210</v>
       </c>
       <c r="M166">
-        <v>51420</v>
+        <v>66.15000000000001</v>
       </c>
     </row>
     <row r="167">
@@ -8223,7 +8130,7 @@
         <v>18351</v>
       </c>
       <c r="M167">
-        <v>51440</v>
+        <v>66.78</v>
       </c>
     </row>
     <row r="168">
@@ -8270,7 +8177,7 @@
         <v>0</v>
       </c>
       <c r="M168">
-        <v>51120</v>
+        <v>63.62</v>
       </c>
     </row>
     <row r="169">
@@ -8317,7 +8224,7 @@
         <v>127348</v>
       </c>
       <c r="M169">
-        <v>51180</v>
+        <v>53.5</v>
       </c>
     </row>
     <row r="170">
@@ -8364,7 +8271,7 @@
         <v>12482</v>
       </c>
       <c r="M170">
-        <v>51430</v>
+        <v>88.34999999999999</v>
       </c>
     </row>
     <row r="171">
@@ -8411,7 +8318,7 @@
         <v>53401</v>
       </c>
       <c r="M171">
-        <v>50260</v>
+        <v>70.53</v>
       </c>
     </row>
     <row r="172">
@@ -8458,7 +8365,7 @@
         <v>178017</v>
       </c>
       <c r="M172">
-        <v>51350</v>
+        <v>62.07</v>
       </c>
     </row>
     <row r="173">
@@ -8505,7 +8412,7 @@
         <v>127798</v>
       </c>
       <c r="M173">
-        <v>52070</v>
+        <v>49.05</v>
       </c>
     </row>
     <row r="174">
@@ -8552,7 +8459,7 @@
         <v>46751</v>
       </c>
       <c r="M174">
-        <v>54390</v>
+        <v>38.67</v>
       </c>
     </row>
     <row r="175">
@@ -8599,7 +8506,7 @@
         <v>120682</v>
       </c>
       <c r="M175">
-        <v>51780</v>
+        <v>49.03</v>
       </c>
     </row>
     <row r="176">
@@ -8646,7 +8553,7 @@
         <v>71305</v>
       </c>
       <c r="M176">
-        <v>52640</v>
+        <v>62.46</v>
       </c>
     </row>
     <row r="177">
@@ -8693,7 +8600,7 @@
         <v>114666</v>
       </c>
       <c r="M177">
-        <v>50730</v>
+        <v>51.89</v>
       </c>
     </row>
     <row r="178">
@@ -8740,7 +8647,7 @@
         <v>210399</v>
       </c>
       <c r="M178">
-        <v>52960</v>
+        <v>40.22</v>
       </c>
     </row>
     <row r="179">
@@ -8787,7 +8694,7 @@
         <v>75962</v>
       </c>
       <c r="M179">
-        <v>51680</v>
+        <v>52.78</v>
       </c>
     </row>
     <row r="180">
@@ -8834,7 +8741,7 @@
         <v>0</v>
       </c>
       <c r="M180">
-        <v>53310</v>
+        <v>52.28</v>
       </c>
     </row>
     <row r="181">
@@ -8881,7 +8788,7 @@
         <v>0</v>
       </c>
       <c r="M181">
-        <v>53310</v>
+        <v>24.58</v>
       </c>
     </row>
     <row r="182">
@@ -8928,7 +8835,7 @@
         <v>32758</v>
       </c>
       <c r="M182">
-        <v>54540</v>
+        <v>49.61</v>
       </c>
     </row>
     <row r="183">
@@ -8975,7 +8882,7 @@
         <v>0</v>
       </c>
       <c r="M183">
-        <v>52170</v>
+        <v>61.79</v>
       </c>
     </row>
     <row r="184">
@@ -9022,7 +8929,7 @@
         <v>0</v>
       </c>
       <c r="M184">
-        <v>50900</v>
+        <v>54.76</v>
       </c>
     </row>
     <row r="185">
@@ -9069,7 +8976,7 @@
         <v>0</v>
       </c>
       <c r="M185">
-        <v>51360</v>
+        <v>78.28</v>
       </c>
     </row>
     <row r="186">
@@ -9116,7 +9023,7 @@
         <v>0</v>
       </c>
       <c r="M186">
-        <v>50650</v>
+        <v>83.31</v>
       </c>
     </row>
     <row r="187">
@@ -9163,7 +9070,7 @@
         <v>275901</v>
       </c>
       <c r="M187">
-        <v>51220</v>
+        <v>45.06</v>
       </c>
     </row>
     <row r="188">
@@ -9210,7 +9117,7 @@
         <v>0</v>
       </c>
       <c r="M188">
-        <v>50740</v>
+        <v>72.34999999999999</v>
       </c>
     </row>
     <row r="189">
@@ -9257,7 +9164,7 @@
         <v>0</v>
       </c>
       <c r="M189">
-        <v>50900</v>
+        <v>69.44</v>
       </c>
     </row>
     <row r="190">
@@ -9304,7 +9211,7 @@
         <v>29174</v>
       </c>
       <c r="M190">
-        <v>50410</v>
+        <v>85.78</v>
       </c>
     </row>
     <row r="191">
@@ -9351,7 +9258,7 @@
         <v>99222</v>
       </c>
       <c r="M191">
-        <v>56870</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="192">
@@ -9398,7 +9305,7 @@
         <v>26283</v>
       </c>
       <c r="M192">
-        <v>57150</v>
+        <v>23.88</v>
       </c>
     </row>
     <row r="193">
@@ -9445,7 +9352,7 @@
         <v>126849</v>
       </c>
       <c r="M193">
-        <v>58410</v>
+        <v>11.72</v>
       </c>
     </row>
     <row r="194">
@@ -9492,7 +9399,7 @@
         <v>475192</v>
       </c>
       <c r="M194">
-        <v>56530</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="195">
@@ -9539,7 +9446,7 @@
         <v>533586</v>
       </c>
       <c r="M195">
-        <v>55710</v>
+        <v>17.31</v>
       </c>
     </row>
     <row r="196">
@@ -9586,7 +9493,7 @@
         <v>49003</v>
       </c>
       <c r="M196">
-        <v>61360</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="197">
@@ -9633,7 +9540,7 @@
         <v>0</v>
       </c>
       <c r="M197">
-        <v>59070</v>
+        <v>4.16</v>
       </c>
     </row>
     <row r="198">
@@ -9680,7 +9587,7 @@
         <v>96805</v>
       </c>
       <c r="M198">
-        <v>56630</v>
+        <v>8.91</v>
       </c>
     </row>
     <row r="199">
@@ -9727,7 +9634,7 @@
         <v>0</v>
       </c>
       <c r="M199">
-        <v>54600</v>
+        <v>25.43</v>
       </c>
     </row>
     <row r="200">
@@ -9774,7 +9681,7 @@
         <v>0</v>
       </c>
       <c r="M200">
-        <v>55150</v>
+        <v>35.05</v>
       </c>
     </row>
     <row r="201">
@@ -9821,7 +9728,7 @@
         <v>0</v>
       </c>
       <c r="M201">
-        <v>58110</v>
+        <v>15.59</v>
       </c>
     </row>
     <row r="202">
@@ -9868,7 +9775,7 @@
         <v>126920</v>
       </c>
       <c r="M202">
-        <v>55020</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="203">
@@ -9915,7 +9822,7 @@
         <v>0</v>
       </c>
       <c r="M203">
-        <v>54420</v>
+        <v>59.54</v>
       </c>
     </row>
     <row r="204">
@@ -9962,7 +9869,7 @@
         <v>0</v>
       </c>
       <c r="M204">
-        <v>52880</v>
+        <v>37.93</v>
       </c>
     </row>
     <row r="205">
@@ -10009,7 +9916,7 @@
         <v>0</v>
       </c>
       <c r="M205">
-        <v>53770</v>
+        <v>44.76</v>
       </c>
     </row>
     <row r="206">
@@ -10056,7 +9963,7 @@
         <v>56905</v>
       </c>
       <c r="M206">
-        <v>55330</v>
+        <v>50.05</v>
       </c>
     </row>
     <row r="207">
@@ -10103,7 +10010,7 @@
         <v>0</v>
       </c>
       <c r="M207">
-        <v>53150</v>
+        <v>100</v>
       </c>
     </row>
     <row r="208">
@@ -10150,7 +10057,7 @@
         <v>163090</v>
       </c>
       <c r="M208">
-        <v>54870</v>
+        <v>32.73</v>
       </c>
     </row>
     <row r="209">
@@ -10197,7 +10104,7 @@
         <v>21278</v>
       </c>
       <c r="M209">
-        <v>56320</v>
+        <v>66.76000000000001</v>
       </c>
     </row>
     <row r="210">
@@ -10244,7 +10151,7 @@
         <v>14107</v>
       </c>
       <c r="M210">
-        <v>53640</v>
+        <v>62.13</v>
       </c>
     </row>
     <row r="211">
@@ -10291,7 +10198,7 @@
         <v>0</v>
       </c>
       <c r="M211">
-        <v>53640</v>
+        <v>70.14</v>
       </c>
     </row>
     <row r="212">
@@ -10338,7 +10245,7 @@
         <v>0</v>
       </c>
       <c r="M212">
-        <v>56590</v>
+        <v>74.31999999999999</v>
       </c>
     </row>
     <row r="213">
@@ -10385,7 +10292,7 @@
         <v>117606</v>
       </c>
       <c r="M213">
-        <v>55150</v>
+        <v>67.05</v>
       </c>
     </row>
     <row r="214">
@@ -10432,7 +10339,7 @@
         <v>52622</v>
       </c>
       <c r="M214">
-        <v>55260</v>
+        <v>32.21</v>
       </c>
     </row>
     <row r="215">
@@ -10479,7 +10386,7 @@
         <v>108590</v>
       </c>
       <c r="M215">
-        <v>56000</v>
+        <v>12.82</v>
       </c>
     </row>
     <row r="216">
@@ -10526,7 +10433,7 @@
         <v>98174</v>
       </c>
       <c r="M216">
-        <v>57440</v>
+        <v>12.06</v>
       </c>
     </row>
     <row r="217">
@@ -10573,7 +10480,7 @@
         <v>136017</v>
       </c>
       <c r="M217">
-        <v>57550</v>
+        <v>4.88</v>
       </c>
     </row>
     <row r="218">
@@ -10620,7 +10527,7 @@
         <v>164097</v>
       </c>
       <c r="M218">
-        <v>55570</v>
+        <v>31.75</v>
       </c>
     </row>
     <row r="219">
@@ -10667,7 +10574,7 @@
         <v>32764</v>
       </c>
       <c r="M219">
-        <v>55290</v>
+        <v>32.12</v>
       </c>
     </row>
     <row r="220">
@@ -10714,7 +10621,7 @@
         <v>0</v>
       </c>
       <c r="M220">
-        <v>56360</v>
+        <v>26.55</v>
       </c>
     </row>
     <row r="221">
@@ -10761,7 +10668,7 @@
         <v>0</v>
       </c>
       <c r="M221">
-        <v>52250</v>
+        <v>60.15</v>
       </c>
     </row>
     <row r="222">
@@ -10808,7 +10715,7 @@
         <v>0</v>
       </c>
       <c r="M222">
-        <v>54230</v>
+        <v>57.85</v>
       </c>
     </row>
     <row r="223">
@@ -10855,7 +10762,7 @@
         <v>0</v>
       </c>
       <c r="M223">
-        <v>54760</v>
+        <v>50.23</v>
       </c>
     </row>
     <row r="224">
@@ -10902,7 +10809,7 @@
         <v>0</v>
       </c>
       <c r="M224">
-        <v>53590</v>
+        <v>45.43</v>
       </c>
     </row>
     <row r="225">
@@ -10949,7 +10856,7 @@
         <v>81604</v>
       </c>
       <c r="M225">
-        <v>57680</v>
+        <v>24.17</v>
       </c>
     </row>
     <row r="226">
@@ -10996,7 +10903,7 @@
         <v>0</v>
       </c>
       <c r="M226">
-        <v>52840</v>
+        <v>44.32</v>
       </c>
     </row>
     <row r="227">
@@ -11043,7 +10950,7 @@
         <v>0</v>
       </c>
       <c r="M227">
-        <v>53620</v>
+        <v>60.93</v>
       </c>
     </row>
     <row r="228">
@@ -11090,7 +10997,7 @@
         <v>0</v>
       </c>
       <c r="M228">
-        <v>51880</v>
+        <v>100</v>
       </c>
     </row>
     <row r="229">
@@ -11137,7 +11044,7 @@
         <v>77107</v>
       </c>
       <c r="M229">
-        <v>52280</v>
+        <v>28.71</v>
       </c>
     </row>
     <row r="230">
@@ -11184,7 +11091,7 @@
         <v>0</v>
       </c>
       <c r="M230">
-        <v>52990</v>
+        <v>48.9</v>
       </c>
     </row>
     <row r="231">
@@ -11231,7 +11138,7 @@
         <v>27190</v>
       </c>
       <c r="M231">
-        <v>54960</v>
+        <v>99.92</v>
       </c>
     </row>
     <row r="232">
@@ -11278,7 +11185,7 @@
         <v>60455</v>
       </c>
       <c r="M232">
-        <v>52300</v>
+        <v>33.04</v>
       </c>
     </row>
     <row r="233">
@@ -11325,7 +11232,7 @@
         <v>0</v>
       </c>
       <c r="M233">
-        <v>52880</v>
+        <v>16.39</v>
       </c>
     </row>
     <row r="234">
@@ -11372,7 +11279,7 @@
         <v>0</v>
       </c>
       <c r="M234">
-        <v>54450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="235">
@@ -11419,7 +11326,7 @@
         <v>0</v>
       </c>
       <c r="M235">
-        <v>53180</v>
+        <v>42.51</v>
       </c>
     </row>
     <row r="236">
@@ -11466,7 +11373,7 @@
         <v>0</v>
       </c>
       <c r="M236">
-        <v>54570</v>
+        <v>86.59999999999999</v>
       </c>
     </row>
     <row r="237">
@@ -11513,7 +11420,7 @@
         <v>0</v>
       </c>
       <c r="M237">
-        <v>54590</v>
+        <v>45.62</v>
       </c>
     </row>
     <row r="238">
@@ -11560,7 +11467,7 @@
         <v>46900</v>
       </c>
       <c r="M238">
-        <v>54920</v>
+        <v>51.79</v>
       </c>
     </row>
     <row r="239">
@@ -11607,7 +11514,7 @@
         <v>2788040</v>
       </c>
       <c r="M239">
-        <v>61420</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="240">
@@ -11654,7 +11561,7 @@
         <v>94159</v>
       </c>
       <c r="M240">
-        <v>56040</v>
+        <v>16.42</v>
       </c>
     </row>
     <row r="241">
@@ -11701,7 +11608,7 @@
         <v>0</v>
       </c>
       <c r="M241">
-        <v>55250</v>
+        <v>53.71</v>
       </c>
     </row>
     <row r="242">
@@ -11748,7 +11655,7 @@
         <v>11071</v>
       </c>
       <c r="M242">
-        <v>57020</v>
+        <v>61.04</v>
       </c>
     </row>
     <row r="243">
@@ -11795,7 +11702,7 @@
         <v>0</v>
       </c>
       <c r="M243">
-        <v>58960</v>
+        <v>38.36</v>
       </c>
     </row>
     <row r="244">
@@ -11842,7 +11749,7 @@
         <v>7810</v>
       </c>
       <c r="M244">
-        <v>58610</v>
+        <v>5.48</v>
       </c>
     </row>
     <row r="245">
@@ -11889,7 +11796,7 @@
         <v>0</v>
       </c>
       <c r="M245">
-        <v>56370</v>
+        <v>43.18</v>
       </c>
     </row>
     <row r="246">
@@ -11936,7 +11843,7 @@
         <v>7592</v>
       </c>
       <c r="M246">
-        <v>59490</v>
+        <v>70.26000000000001</v>
       </c>
     </row>
     <row r="247">
@@ -11983,7 +11890,7 @@
         <v>0</v>
       </c>
       <c r="M247">
-        <v>56890</v>
+        <v>34.8</v>
       </c>
     </row>
     <row r="248">
@@ -12030,7 +11937,7 @@
         <v>352251</v>
       </c>
       <c r="M248">
-        <v>55340</v>
+        <v>30.83</v>
       </c>
     </row>
     <row r="249">
@@ -12077,7 +11984,7 @@
         <v>70757</v>
       </c>
       <c r="M249">
-        <v>55840</v>
+        <v>40.7</v>
       </c>
     </row>
     <row r="250">
@@ -12124,7 +12031,7 @@
         <v>46571</v>
       </c>
       <c r="M250">
-        <v>53470</v>
+        <v>51.24</v>
       </c>
     </row>
     <row r="251">
@@ -12171,7 +12078,7 @@
         <v>370144</v>
       </c>
       <c r="M251">
-        <v>54940</v>
+        <v>37.03</v>
       </c>
     </row>
     <row r="252">
@@ -12218,7 +12125,7 @@
         <v>0</v>
       </c>
       <c r="M252">
-        <v>56990</v>
+        <v>29.17</v>
       </c>
     </row>
     <row r="253">
@@ -12265,7 +12172,7 @@
         <v>0</v>
       </c>
       <c r="M253">
-        <v>56840</v>
+        <v>57.59</v>
       </c>
     </row>
     <row r="254">
@@ -12312,7 +12219,7 @@
         <v>8728</v>
       </c>
       <c r="M254">
-        <v>58560</v>
+        <v>22.79</v>
       </c>
     </row>
     <row r="255">
@@ -12359,7 +12266,7 @@
         <v>0</v>
       </c>
       <c r="M255">
-        <v>59370</v>
+        <v>52.74</v>
       </c>
     </row>
     <row r="256">
@@ -12406,7 +12313,7 @@
         <v>19269</v>
       </c>
       <c r="M256">
-        <v>58580</v>
+        <v>22.58</v>
       </c>
     </row>
     <row r="257">
@@ -12453,7 +12360,7 @@
         <v>0</v>
       </c>
       <c r="M257">
-        <v>58770</v>
+        <v>9.09</v>
       </c>
     </row>
     <row r="258">
@@ -12500,7 +12407,7 @@
         <v>0</v>
       </c>
       <c r="M258">
-        <v>54950</v>
+        <v>25.99</v>
       </c>
     </row>
     <row r="259">
@@ -12547,7 +12454,7 @@
         <v>0</v>
       </c>
       <c r="M259">
-        <v>53640</v>
+        <v>99.73999999999999</v>
       </c>
     </row>
     <row r="260">
@@ -12594,7 +12501,7 @@
         <v>0</v>
       </c>
       <c r="M260">
-        <v>53920</v>
+        <v>47.93</v>
       </c>
     </row>
     <row r="261">
@@ -12641,7 +12548,7 @@
         <v>25652</v>
       </c>
       <c r="M261">
-        <v>57710</v>
+        <v>40.57</v>
       </c>
     </row>
     <row r="262">
@@ -12688,7 +12595,7 @@
         <v>0</v>
       </c>
       <c r="M262">
-        <v>58850</v>
+        <v>62.17</v>
       </c>
     </row>
     <row r="263">
@@ -12735,7 +12642,7 @@
         <v>0</v>
       </c>
       <c r="M263">
-        <v>61200</v>
+        <v>24.66</v>
       </c>
     </row>
     <row r="264">
@@ -12782,7 +12689,7 @@
         <v>0</v>
       </c>
       <c r="M264">
-        <v>55350</v>
+        <v>100</v>
       </c>
     </row>
     <row r="265">
@@ -12829,7 +12736,7 @@
         <v>17626</v>
       </c>
       <c r="M265">
-        <v>54720</v>
+        <v>71.84</v>
       </c>
     </row>
     <row r="266">
@@ -12876,7 +12783,7 @@
         <v>0</v>
       </c>
       <c r="M266">
-        <v>54650</v>
+        <v>62.13</v>
       </c>
     </row>
     <row r="267">
@@ -12923,7 +12830,7 @@
         <v>4203</v>
       </c>
       <c r="M267">
-        <v>53530</v>
+        <v>99.68000000000001</v>
       </c>
     </row>
     <row r="268">
@@ -12970,7 +12877,7 @@
         <v>0</v>
       </c>
       <c r="M268">
-        <v>55790</v>
+        <v>36.04</v>
       </c>
     </row>
     <row r="269">
@@ -13017,7 +12924,7 @@
         <v>25193</v>
       </c>
       <c r="M269">
-        <v>53770</v>
+        <v>52.06</v>
       </c>
     </row>
     <row r="270">
@@ -13064,7 +12971,7 @@
         <v>246632</v>
       </c>
       <c r="M270">
-        <v>54650</v>
+        <v>23.13</v>
       </c>
     </row>
     <row r="271">
@@ -13111,7 +13018,7 @@
         <v>264919</v>
       </c>
       <c r="M271">
-        <v>52480</v>
+        <v>39.17</v>
       </c>
     </row>
     <row r="272">
@@ -13158,7 +13065,7 @@
         <v>91891</v>
       </c>
       <c r="M272">
-        <v>53940</v>
+        <v>45.56</v>
       </c>
     </row>
     <row r="273">
@@ -13205,7 +13112,7 @@
         <v>0</v>
       </c>
       <c r="M273">
-        <v>58990</v>
+        <v>5.94</v>
       </c>
     </row>
     <row r="274">
@@ -13252,7 +13159,7 @@
         <v>142297</v>
       </c>
       <c r="M274">
-        <v>52630</v>
+        <v>54.24</v>
       </c>
     </row>
     <row r="275">
@@ -13299,7 +13206,7 @@
         <v>3718</v>
       </c>
       <c r="M275">
-        <v>54690</v>
+        <v>75.45</v>
       </c>
     </row>
     <row r="276">
@@ -13346,7 +13253,7 @@
         <v>0</v>
       </c>
       <c r="M276">
-        <v>55100</v>
+        <v>47.3</v>
       </c>
     </row>
     <row r="277">
@@ -13393,7 +13300,7 @@
         <v>199489</v>
       </c>
       <c r="M277">
-        <v>55730</v>
+        <v>30.98</v>
       </c>
     </row>
     <row r="278">
@@ -13440,7 +13347,7 @@
         <v>0</v>
       </c>
       <c r="M278">
-        <v>54370</v>
+        <v>55.34</v>
       </c>
     </row>
     <row r="279">
@@ -13487,7 +13394,7 @@
         <v>0</v>
       </c>
       <c r="M279">
-        <v>53940</v>
+        <v>45.93</v>
       </c>
     </row>
     <row r="280">
@@ -13534,7 +13441,7 @@
         <v>33133</v>
       </c>
       <c r="M280">
-        <v>53840</v>
+        <v>50.37</v>
       </c>
     </row>
     <row r="281">
@@ -13581,7 +13488,7 @@
         <v>341705</v>
       </c>
       <c r="M281">
-        <v>51000</v>
+        <v>46.24</v>
       </c>
     </row>
     <row r="282">
@@ -13597,7 +13504,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D282">
@@ -13621,14 +13528,11 @@
       <c r="J282">
         <v>0.2315682892224986</v>
       </c>
-      <c r="K282">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L282">
         <v>1278554</v>
       </c>
       <c r="M282">
-        <v>60880</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283">
@@ -13644,7 +13548,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D283">
@@ -13668,14 +13572,11 @@
       <c r="J283">
         <v>0.3563970951281953</v>
       </c>
-      <c r="K283">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L283">
         <v>26292</v>
       </c>
       <c r="M283">
-        <v>54010</v>
+        <v>32.91</v>
       </c>
     </row>
     <row r="284">
@@ -13691,7 +13592,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D284">
@@ -13715,14 +13616,11 @@
       <c r="J284">
         <v>0.3812735850844319</v>
       </c>
-      <c r="K284">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L284">
         <v>24688</v>
       </c>
       <c r="M284">
-        <v>55400</v>
+        <v>27.05</v>
       </c>
     </row>
     <row r="285">
@@ -13738,7 +13636,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D285">
@@ -13762,14 +13660,11 @@
       <c r="J285">
         <v>0.2316106446318464</v>
       </c>
-      <c r="K285">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L285">
         <v>0</v>
       </c>
       <c r="M285">
-        <v>54870</v>
+        <v>66.53</v>
       </c>
     </row>
     <row r="286">
@@ -13785,7 +13680,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D286">
@@ -13809,14 +13704,11 @@
       <c r="J286">
         <v>40.16124405499531</v>
       </c>
-      <c r="K286">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L286">
         <v>0</v>
       </c>
       <c r="M286">
-        <v>51780</v>
+        <v>99.89</v>
       </c>
     </row>
     <row r="287">
@@ -13832,7 +13724,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D287">
@@ -13856,14 +13748,11 @@
       <c r="J287">
         <v>0.1438713589994311</v>
       </c>
-      <c r="K287">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L287">
         <v>0</v>
       </c>
       <c r="M287">
-        <v>53330</v>
+        <v>37.2</v>
       </c>
     </row>
     <row r="288">
@@ -13879,7 +13768,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D288">
@@ -13903,14 +13792,11 @@
       <c r="J288">
         <v>28.19494477479097</v>
       </c>
-      <c r="K288">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L288">
         <v>0</v>
       </c>
       <c r="M288">
-        <v>50190</v>
+        <v>59.54</v>
       </c>
     </row>
     <row r="289">
@@ -13926,7 +13812,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D289">
@@ -13950,14 +13836,11 @@
       <c r="J289">
         <v>0.3432629468001519</v>
       </c>
-      <c r="K289">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L289">
         <v>0</v>
       </c>
       <c r="M289">
-        <v>52180</v>
+        <v>31.19</v>
       </c>
     </row>
     <row r="290">
@@ -13973,7 +13856,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D290">
@@ -13997,14 +13880,11 @@
       <c r="J290">
         <v>30.12950947722824</v>
       </c>
-      <c r="K290">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L290">
         <v>0</v>
       </c>
       <c r="M290">
-        <v>52490</v>
+        <v>69.29000000000001</v>
       </c>
     </row>
     <row r="291">
@@ -14020,7 +13900,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D291">
@@ -14044,14 +13924,11 @@
       <c r="J291">
         <v>1.296233999884783</v>
       </c>
-      <c r="K291">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L291">
         <v>0</v>
       </c>
       <c r="M291">
-        <v>52010</v>
+        <v>57.43</v>
       </c>
     </row>
     <row r="292">
@@ -14067,7 +13944,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D292">
@@ -14091,14 +13968,11 @@
       <c r="J292">
         <v>0.3794304793144223</v>
       </c>
-      <c r="K292">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L292">
         <v>24917</v>
       </c>
       <c r="M292">
-        <v>55570</v>
+        <v>34.39</v>
       </c>
     </row>
     <row r="293">
@@ -14114,7 +13988,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D293">
@@ -14138,14 +14012,11 @@
       <c r="J293">
         <v>5.542966561887937</v>
       </c>
-      <c r="K293">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L293">
         <v>0</v>
       </c>
       <c r="M293">
-        <v>56450</v>
+        <v>33.68</v>
       </c>
     </row>
     <row r="294">
@@ -14161,7 +14032,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D294">
@@ -14185,14 +14056,11 @@
       <c r="J294">
         <v>2.213948002214585</v>
       </c>
-      <c r="K294">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L294">
         <v>0</v>
       </c>
       <c r="M294">
-        <v>61200</v>
+        <v>11.93</v>
       </c>
     </row>
     <row r="295">
@@ -14208,7 +14076,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D295">
@@ -14232,14 +14100,11 @@
       <c r="J295">
         <v>0.1853509962461325</v>
       </c>
-      <c r="K295">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L295">
         <v>0</v>
       </c>
       <c r="M295">
-        <v>53460</v>
+        <v>67.91</v>
       </c>
     </row>
     <row r="296">
@@ -14255,7 +14120,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D296">
@@ -14279,14 +14144,11 @@
       <c r="J296">
         <v>36.32222499731586</v>
       </c>
-      <c r="K296">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L296">
         <v>12411</v>
       </c>
       <c r="M296">
-        <v>55470</v>
+        <v>100</v>
       </c>
     </row>
     <row r="297">
@@ -14302,7 +14164,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D297">
@@ -14326,14 +14188,11 @@
       <c r="J297">
         <v>41.39691448249086</v>
       </c>
-      <c r="K297">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L297">
         <v>0</v>
       </c>
       <c r="M297">
-        <v>51080</v>
+        <v>57.33</v>
       </c>
     </row>
     <row r="298">
@@ -14349,7 +14208,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D298">
@@ -14373,14 +14232,11 @@
       <c r="J298">
         <v>0.3115826552877649</v>
       </c>
-      <c r="K298">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L298">
         <v>269923</v>
       </c>
       <c r="M298">
-        <v>57150</v>
+        <v>27.01</v>
       </c>
     </row>
     <row r="299">
@@ -14396,7 +14252,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D299">
@@ -14420,14 +14276,11 @@
       <c r="J299">
         <v>0.1071880455514616</v>
       </c>
-      <c r="K299">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L299">
         <v>78552</v>
       </c>
       <c r="M299">
-        <v>51120</v>
+        <v>99.84999999999999</v>
       </c>
     </row>
     <row r="300">
@@ -14443,7 +14296,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D300">
@@ -14467,14 +14320,11 @@
       <c r="J300">
         <v>0.3860790644001836</v>
       </c>
-      <c r="K300">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L300">
         <v>0</v>
       </c>
       <c r="M300">
-        <v>55620</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="301">
@@ -14490,7 +14340,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D301">
@@ -14514,14 +14364,11 @@
       <c r="J301">
         <v>0.3610894756160769</v>
       </c>
-      <c r="K301">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L301">
         <v>47166</v>
       </c>
       <c r="M301">
-        <v>53770</v>
+        <v>29.89</v>
       </c>
     </row>
     <row r="302">
@@ -14537,7 +14384,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D302">
@@ -14561,14 +14408,11 @@
       <c r="J302">
         <v>24.54082546958647</v>
       </c>
-      <c r="K302">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L302">
         <v>0</v>
       </c>
       <c r="M302">
-        <v>51840</v>
+        <v>68.87</v>
       </c>
     </row>
     <row r="303">
@@ -14584,7 +14428,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D303">
@@ -14608,14 +14452,11 @@
       <c r="J303">
         <v>61.31517863667393</v>
       </c>
-      <c r="K303">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L303">
         <v>2280</v>
       </c>
       <c r="M303">
-        <v>51970</v>
+        <v>83.09</v>
       </c>
     </row>
     <row r="304">
@@ -14631,7 +14472,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D304">
@@ -14655,14 +14496,11 @@
       <c r="J304">
         <v>75.67484654329289</v>
       </c>
-      <c r="K304">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L304">
         <v>0</v>
       </c>
       <c r="M304">
-        <v>52170</v>
+        <v>47.75</v>
       </c>
     </row>
     <row r="305">
@@ -14678,7 +14516,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D305">
@@ -14702,14 +14540,11 @@
       <c r="J305">
         <v>65.2200782971381</v>
       </c>
-      <c r="K305">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L305">
         <v>14363</v>
       </c>
       <c r="M305">
-        <v>51960</v>
+        <v>72.72</v>
       </c>
     </row>
     <row r="306">
@@ -14725,7 +14560,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D306">
@@ -14749,14 +14584,11 @@
       <c r="J306">
         <v>0.18229686884876</v>
       </c>
-      <c r="K306">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L306">
         <v>21962</v>
       </c>
       <c r="M306">
-        <v>52880</v>
+        <v>53.06</v>
       </c>
     </row>
     <row r="307">
@@ -14772,7 +14604,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D307">
@@ -14796,14 +14628,11 @@
       <c r="J307">
         <v>18.165499124931</v>
       </c>
-      <c r="K307">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L307">
         <v>0</v>
       </c>
       <c r="M307">
-        <v>52770</v>
+        <v>69.72</v>
       </c>
     </row>
     <row r="308">
@@ -14819,7 +14648,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D308">
@@ -14843,14 +14672,11 @@
       <c r="J308">
         <v>17.90832820202273</v>
       </c>
-      <c r="K308">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L308">
         <v>3064</v>
       </c>
       <c r="M308">
-        <v>54190</v>
+        <v>50.2</v>
       </c>
     </row>
     <row r="309">
@@ -14866,7 +14692,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D309">
@@ -14890,14 +14716,11 @@
       <c r="J309">
         <v>28.83796633385532</v>
       </c>
-      <c r="K309">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L309">
         <v>12440</v>
       </c>
       <c r="M309">
-        <v>53610</v>
+        <v>52.51</v>
       </c>
     </row>
     <row r="310">
@@ -14913,7 +14736,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D310">
@@ -14937,14 +14760,11 @@
       <c r="J310">
         <v>25.71915897389005</v>
       </c>
-      <c r="K310">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L310">
         <v>14480</v>
       </c>
       <c r="M310">
-        <v>53550</v>
+        <v>99.5</v>
       </c>
     </row>
     <row r="311">
@@ -14960,7 +14780,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D311">
@@ -14984,14 +14804,11 @@
       <c r="J311">
         <v>0.5078991917759708</v>
       </c>
-      <c r="K311">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L311">
         <v>0</v>
       </c>
       <c r="M311">
-        <v>54800</v>
+        <v>53.57</v>
       </c>
     </row>
     <row r="312">
@@ -15007,7 +14824,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D312">
@@ -15031,14 +14848,11 @@
       <c r="J312">
         <v>0.1713157195221743</v>
       </c>
-      <c r="K312">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L312">
         <v>0</v>
       </c>
       <c r="M312">
-        <v>52970</v>
+        <v>60.74</v>
       </c>
     </row>
     <row r="313">
@@ -15054,7 +14868,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D313">
@@ -15078,14 +14892,11 @@
       <c r="J313">
         <v>0.001737111854873408</v>
       </c>
-      <c r="K313">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L313">
         <v>20967</v>
       </c>
       <c r="M313">
-        <v>55360</v>
+        <v>53.93</v>
       </c>
     </row>
     <row r="314">
@@ -15101,7 +14912,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D314">
@@ -15125,14 +14936,11 @@
       <c r="J314">
         <v>0.1511213078816971</v>
       </c>
-      <c r="K314">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L314">
         <v>77464</v>
       </c>
       <c r="M314">
-        <v>53940</v>
+        <v>64.72</v>
       </c>
     </row>
     <row r="315">
@@ -15148,7 +14956,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D315">
@@ -15172,14 +14980,11 @@
       <c r="J315">
         <v>0.1222331099894117</v>
       </c>
-      <c r="K315">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L315">
         <v>20814</v>
       </c>
       <c r="M315">
-        <v>56410</v>
+        <v>47.68</v>
       </c>
     </row>
     <row r="316">
@@ -15195,7 +15000,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D316">
@@ -15219,14 +15024,11 @@
       <c r="J316">
         <v>0.1662148061744048</v>
       </c>
-      <c r="K316">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L316">
         <v>34196</v>
       </c>
       <c r="M316">
-        <v>53690</v>
+        <v>68.03</v>
       </c>
     </row>
     <row r="317">
@@ -15242,7 +15044,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>SØR-TRØNDELAG</t>
         </is>
       </c>
       <c r="D317">
@@ -15266,14 +15068,11 @@
       <c r="J317">
         <v>0.290013456336721</v>
       </c>
-      <c r="K317">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L317">
         <v>43884</v>
       </c>
       <c r="M317">
-        <v>53810</v>
+        <v>35.41</v>
       </c>
     </row>
     <row r="318">
@@ -15289,7 +15088,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>NORD-TRØNDELAG</t>
         </is>
       </c>
       <c r="D318">
@@ -15313,14 +15112,11 @@
       <c r="J318">
         <v>0.1672469212363001</v>
       </c>
-      <c r="K318">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L318">
         <v>16210</v>
       </c>
       <c r="M318">
-        <v>55510</v>
+        <v>41.84</v>
       </c>
     </row>
     <row r="319">
@@ -15336,7 +15132,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>TrC8ndelag</t>
         </is>
       </c>
       <c r="D319">
@@ -15360,14 +15156,11 @@
       <c r="J319">
         <v>26.01845859168469</v>
       </c>
-      <c r="K319">
-        <v>58.06874999999999</v>
-      </c>
       <c r="L319">
         <v>0</v>
       </c>
       <c r="M319">
-        <v>52170</v>
+        <v>62.92</v>
       </c>
     </row>
     <row r="320">
@@ -15414,7 +15207,7 @@
         <v>1184871</v>
       </c>
       <c r="M320">
-        <v>58230</v>
+        <v>8.779999999999999</v>
       </c>
     </row>
     <row r="321">
@@ -15461,7 +15254,7 @@
         <v>174436</v>
       </c>
       <c r="M321">
-        <v>57230</v>
+        <v>14.28</v>
       </c>
     </row>
     <row r="322">
@@ -15508,7 +15301,7 @@
         <v>0</v>
       </c>
       <c r="M322">
-        <v>53710</v>
+        <v>37.29</v>
       </c>
     </row>
     <row r="323">
@@ -15555,7 +15348,7 @@
         <v>0</v>
       </c>
       <c r="M323">
-        <v>55050</v>
+        <v>61.46</v>
       </c>
     </row>
     <row r="324">
@@ -15602,7 +15395,7 @@
         <v>0</v>
       </c>
       <c r="M324">
-        <v>54030</v>
+        <v>64.68000000000001</v>
       </c>
     </row>
     <row r="325">
@@ -15649,7 +15442,7 @@
         <v>0</v>
       </c>
       <c r="M325">
-        <v>50900</v>
+        <v>100</v>
       </c>
     </row>
     <row r="326">
@@ -15696,7 +15489,7 @@
         <v>10128</v>
       </c>
       <c r="M326">
-        <v>51250</v>
+        <v>69.56999999999999</v>
       </c>
     </row>
     <row r="327">
@@ -15743,7 +15536,7 @@
         <v>7826</v>
       </c>
       <c r="M327">
-        <v>56320</v>
+        <v>36.25</v>
       </c>
     </row>
     <row r="328">
@@ -15790,7 +15583,7 @@
         <v>0</v>
       </c>
       <c r="M328">
-        <v>53810</v>
+        <v>61.58</v>
       </c>
     </row>
     <row r="329">
@@ -15837,7 +15630,7 @@
         <v>16898</v>
       </c>
       <c r="M329">
-        <v>54860</v>
+        <v>42.51</v>
       </c>
     </row>
     <row r="330">
@@ -15884,7 +15677,7 @@
         <v>10923</v>
       </c>
       <c r="M330">
-        <v>54200</v>
+        <v>44.13</v>
       </c>
     </row>
     <row r="331">
@@ -15931,7 +15724,7 @@
         <v>8315</v>
       </c>
       <c r="M331">
-        <v>52450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="332">
@@ -15978,7 +15771,7 @@
         <v>154744</v>
       </c>
       <c r="M332">
-        <v>53670</v>
+        <v>45.88</v>
       </c>
     </row>
     <row r="333">
@@ -16025,7 +15818,7 @@
         <v>0</v>
       </c>
       <c r="M333">
-        <v>52580</v>
+        <v>70.56</v>
       </c>
     </row>
     <row r="334">
@@ -16072,7 +15865,7 @@
         <v>14714</v>
       </c>
       <c r="M334">
-        <v>50870</v>
+        <v>76.75</v>
       </c>
     </row>
     <row r="335">
@@ -16119,7 +15912,7 @@
         <v>18449</v>
       </c>
       <c r="M335">
-        <v>52340</v>
+        <v>63.62</v>
       </c>
     </row>
     <row r="336">
@@ -16166,7 +15959,7 @@
         <v>60955</v>
       </c>
       <c r="M336">
-        <v>51460</v>
+        <v>70.41</v>
       </c>
     </row>
     <row r="337">
@@ -16213,7 +16006,7 @@
         <v>0</v>
       </c>
       <c r="M337">
-        <v>53390</v>
+        <v>72.95</v>
       </c>
     </row>
     <row r="338">
@@ -16260,7 +16053,7 @@
         <v>18994</v>
       </c>
       <c r="M338">
-        <v>52640</v>
+        <v>12.03</v>
       </c>
     </row>
     <row r="339">
@@ -16307,7 +16100,7 @@
         <v>10439</v>
       </c>
       <c r="M339">
-        <v>53880</v>
+        <v>42.8</v>
       </c>
     </row>
     <row r="340">
@@ -16354,7 +16147,7 @@
         <v>12189</v>
       </c>
       <c r="M340">
-        <v>53350</v>
+        <v>64.13</v>
       </c>
     </row>
     <row r="341">
@@ -16401,7 +16194,7 @@
         <v>223353</v>
       </c>
       <c r="M341">
-        <v>55570</v>
+        <v>17.38</v>
       </c>
     </row>
     <row r="342">
@@ -16448,7 +16241,7 @@
         <v>109594</v>
       </c>
       <c r="M342">
-        <v>57600</v>
+        <v>10.78</v>
       </c>
     </row>
     <row r="343">
@@ -16495,7 +16288,7 @@
         <v>11341</v>
       </c>
       <c r="M343">
-        <v>55160</v>
+        <v>19.84</v>
       </c>
     </row>
     <row r="344">
@@ -16542,7 +16335,7 @@
         <v>11696</v>
       </c>
       <c r="M344">
-        <v>55640</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="345">
@@ -16589,7 +16382,7 @@
         <v>0</v>
       </c>
       <c r="M345">
-        <v>53120</v>
+        <v>29.63</v>
       </c>
     </row>
     <row r="346">
@@ -16636,7 +16429,7 @@
         <v>0</v>
       </c>
       <c r="M346">
-        <v>52500</v>
+        <v>47.75</v>
       </c>
     </row>
     <row r="347">
@@ -16683,7 +16476,7 @@
         <v>18604</v>
       </c>
       <c r="M347">
-        <v>50540</v>
+        <v>43.29</v>
       </c>
     </row>
     <row r="348">
@@ -16730,7 +16523,7 @@
         <v>0</v>
       </c>
       <c r="M348">
-        <v>49500</v>
+        <v>31.56</v>
       </c>
     </row>
     <row r="349">
@@ -16777,7 +16570,7 @@
         <v>0</v>
       </c>
       <c r="M349">
-        <v>50620</v>
+        <v>17.43</v>
       </c>
     </row>
     <row r="350">
@@ -16824,7 +16617,7 @@
         <v>107475</v>
       </c>
       <c r="M350">
-        <v>52840</v>
+        <v>9.93</v>
       </c>
     </row>
     <row r="351">
@@ -16871,7 +16664,7 @@
         <v>32815</v>
       </c>
       <c r="M351">
-        <v>54400</v>
+        <v>42.07</v>
       </c>
     </row>
     <row r="352">
@@ -16918,7 +16711,7 @@
         <v>0</v>
       </c>
       <c r="M352">
-        <v>52140</v>
+        <v>30.86</v>
       </c>
     </row>
     <row r="353">
@@ -16965,7 +16758,7 @@
         <v>0</v>
       </c>
       <c r="M353">
-        <v>49620</v>
+        <v>12.34</v>
       </c>
     </row>
     <row r="354">
@@ -17012,7 +16805,7 @@
         <v>5990</v>
       </c>
       <c r="M354">
-        <v>52700</v>
+        <v>73.34999999999999</v>
       </c>
     </row>
     <row r="355">
@@ -17059,7 +16852,7 @@
         <v>0</v>
       </c>
       <c r="M355">
-        <v>50840</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="356">
@@ -17106,7 +16899,7 @@
         <v>0</v>
       </c>
       <c r="M356">
-        <v>49730</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="357">
@@ -17153,7 +16946,7 @@
         <v>0</v>
       </c>
       <c r="M357">
-        <v>52250</v>
+        <v>10.09</v>
       </c>
     </row>
     <row r="358">
@@ -17200,7 +16993,7 @@
         <v>0</v>
       </c>
       <c r="M358">
-        <v>52820</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full variable merge data update
</commit_message>
<xml_diff>
--- a/Data/Vinmonopolet/B&R_data.xlsx
+++ b/Data/Vinmonopolet/B&R_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M358"/>
+  <dimension ref="A1:N358"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,6 +420,11 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Monthly_salary</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>prop_spread</t>
         </is>
       </c>
@@ -468,6 +473,9 @@
         <v>6718960</v>
       </c>
       <c r="M2">
+        <v>65900</v>
+      </c>
+      <c r="N2">
         <v>0.23</v>
       </c>
     </row>
@@ -515,6 +523,9 @@
         <v>0</v>
       </c>
       <c r="M3">
+        <v>57360</v>
+      </c>
+      <c r="N3">
         <v>16.57</v>
       </c>
     </row>
@@ -562,6 +573,9 @@
         <v>1160696</v>
       </c>
       <c r="M4">
+        <v>68170</v>
+      </c>
+      <c r="N4">
         <v>4</v>
       </c>
     </row>
@@ -609,6 +623,9 @@
         <v>254352</v>
       </c>
       <c r="M5">
+        <v>59760</v>
+      </c>
+      <c r="N5">
         <v>1.94</v>
       </c>
     </row>
@@ -656,6 +673,9 @@
         <v>234743</v>
       </c>
       <c r="M6">
+        <v>62030</v>
+      </c>
+      <c r="N6">
         <v>5.41</v>
       </c>
     </row>
@@ -703,6 +723,9 @@
         <v>0</v>
       </c>
       <c r="M7">
+        <v>55420</v>
+      </c>
+      <c r="N7">
         <v>28.17</v>
       </c>
     </row>
@@ -750,6 +773,9 @@
         <v>0</v>
       </c>
       <c r="M8">
+        <v>52850</v>
+      </c>
+      <c r="N8">
         <v>37.72</v>
       </c>
     </row>
@@ -797,6 +823,9 @@
         <v>6540</v>
       </c>
       <c r="M9">
+        <v>55250</v>
+      </c>
+      <c r="N9">
         <v>45.64</v>
       </c>
     </row>
@@ -844,6 +873,9 @@
         <v>0</v>
       </c>
       <c r="M10">
+        <v>54250</v>
+      </c>
+      <c r="N10">
         <v>19.32</v>
       </c>
     </row>
@@ -891,6 +923,9 @@
         <v>0</v>
       </c>
       <c r="M11">
+        <v>57680</v>
+      </c>
+      <c r="N11">
         <v>17.26</v>
       </c>
     </row>
@@ -938,6 +973,9 @@
         <v>0</v>
       </c>
       <c r="M12">
+        <v>59110</v>
+      </c>
+      <c r="N12">
         <v>11.19</v>
       </c>
     </row>
@@ -985,6 +1023,9 @@
         <v>0</v>
       </c>
       <c r="M13">
+        <v>56490</v>
+      </c>
+      <c r="N13">
         <v>9.93</v>
       </c>
     </row>
@@ -1032,6 +1073,9 @@
         <v>232445</v>
       </c>
       <c r="M14">
+        <v>67920</v>
+      </c>
+      <c r="N14">
         <v>9.359999999999999</v>
       </c>
     </row>
@@ -1079,6 +1123,9 @@
         <v>0</v>
       </c>
       <c r="M15">
+        <v>63280</v>
+      </c>
+      <c r="N15">
         <v>12.4</v>
       </c>
     </row>
@@ -1126,6 +1173,9 @@
         <v>97415</v>
       </c>
       <c r="M16">
+        <v>58520</v>
+      </c>
+      <c r="N16">
         <v>18.04</v>
       </c>
     </row>
@@ -1173,6 +1223,9 @@
         <v>0</v>
       </c>
       <c r="M17">
+        <v>55800</v>
+      </c>
+      <c r="N17">
         <v>76.69</v>
       </c>
     </row>
@@ -1220,6 +1273,9 @@
         <v>51366</v>
       </c>
       <c r="M18">
+        <v>54500</v>
+      </c>
+      <c r="N18">
         <v>68.68000000000001</v>
       </c>
     </row>
@@ -1267,6 +1323,9 @@
         <v>0</v>
       </c>
       <c r="M19">
+        <v>56550</v>
+      </c>
+      <c r="N19">
         <v>8.33</v>
       </c>
     </row>
@@ -1314,6 +1373,9 @@
         <v>0</v>
       </c>
       <c r="M20">
+        <v>59460</v>
+      </c>
+      <c r="N20">
         <v>26.84</v>
       </c>
     </row>
@@ -1361,6 +1423,9 @@
         <v>0</v>
       </c>
       <c r="M21">
+        <v>59670</v>
+      </c>
+      <c r="N21">
         <v>43.26</v>
       </c>
     </row>
@@ -1408,6 +1473,9 @@
         <v>27668</v>
       </c>
       <c r="M22">
+        <v>58920</v>
+      </c>
+      <c r="N22">
         <v>37.08</v>
       </c>
     </row>
@@ -1455,6 +1523,9 @@
         <v>12914</v>
       </c>
       <c r="M23">
+        <v>58220</v>
+      </c>
+      <c r="N23">
         <v>11.44</v>
       </c>
     </row>
@@ -1502,6 +1573,9 @@
         <v>0</v>
       </c>
       <c r="M24">
+        <v>63170</v>
+      </c>
+      <c r="N24">
         <v>100</v>
       </c>
     </row>
@@ -1549,6 +1623,9 @@
         <v>19798</v>
       </c>
       <c r="M25">
+        <v>55890</v>
+      </c>
+      <c r="N25">
         <v>54.75</v>
       </c>
     </row>
@@ -1565,7 +1642,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D26">
@@ -1589,10 +1666,16 @@
       <c r="J26">
         <v>0.2423966295353834</v>
       </c>
+      <c r="K26">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L26">
         <v>158591</v>
       </c>
       <c r="M26">
+        <v>57120</v>
+      </c>
+      <c r="N26">
         <v>8.640000000000001</v>
       </c>
     </row>
@@ -1609,7 +1692,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D27">
@@ -1633,10 +1716,16 @@
       <c r="J27">
         <v>1.22065478644859</v>
       </c>
+      <c r="K27">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L27">
         <v>225946</v>
       </c>
       <c r="M27">
+        <v>57800</v>
+      </c>
+      <c r="N27">
         <v>17.25</v>
       </c>
     </row>
@@ -1653,7 +1742,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D28">
@@ -1677,10 +1766,16 @@
       <c r="J28">
         <v>0.02974320608000384</v>
       </c>
+      <c r="K28">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L28">
         <v>421789</v>
       </c>
       <c r="M28">
+        <v>58100</v>
+      </c>
+      <c r="N28">
         <v>6.97</v>
       </c>
     </row>
@@ -1697,7 +1792,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D29">
@@ -1721,10 +1816,16 @@
       <c r="J29">
         <v>0.1095759996931654</v>
       </c>
+      <c r="K29">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
+        <v>56310</v>
+      </c>
+      <c r="N29">
         <v>83.94</v>
       </c>
     </row>
@@ -1741,7 +1842,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D30">
@@ -1772,6 +1873,9 @@
         <v>0</v>
       </c>
       <c r="M30">
+        <v>55350</v>
+      </c>
+      <c r="N30">
         <v>52.05</v>
       </c>
     </row>
@@ -1788,7 +1892,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D31">
@@ -1812,10 +1916,16 @@
       <c r="J31">
         <v>0.1310903619924779</v>
       </c>
+      <c r="K31">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L31">
         <v>27968</v>
       </c>
       <c r="M31">
+        <v>57490</v>
+      </c>
+      <c r="N31">
         <v>32.33</v>
       </c>
     </row>
@@ -1832,7 +1942,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D32">
@@ -1856,10 +1966,16 @@
       <c r="J32">
         <v>0.2212560507591561</v>
       </c>
+      <c r="K32">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L32">
         <v>0</v>
       </c>
       <c r="M32">
+        <v>59950</v>
+      </c>
+      <c r="N32">
         <v>16.31</v>
       </c>
     </row>
@@ -1876,7 +1992,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D33">
@@ -1907,6 +2023,9 @@
         <v>0</v>
       </c>
       <c r="M33">
+        <v>55420</v>
+      </c>
+      <c r="N33">
         <v>11.67</v>
       </c>
     </row>
@@ -1923,7 +2042,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D34">
@@ -1947,10 +2066,16 @@
       <c r="J34">
         <v>0.332077970727406</v>
       </c>
+      <c r="K34">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L34">
         <v>60697</v>
       </c>
       <c r="M34">
+        <v>54120</v>
+      </c>
+      <c r="N34">
         <v>26.83</v>
       </c>
     </row>
@@ -1967,7 +2092,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D35">
@@ -1991,10 +2116,16 @@
       <c r="J35">
         <v>0.04812428799808574</v>
       </c>
+      <c r="K35">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L35">
         <v>253196</v>
       </c>
       <c r="M35">
+        <v>51840</v>
+      </c>
+      <c r="N35">
         <v>35.33</v>
       </c>
     </row>
@@ -2011,7 +2142,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D36">
@@ -2035,10 +2166,16 @@
       <c r="J36">
         <v>0.3492938422089224</v>
       </c>
+      <c r="K36">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L36">
         <v>0</v>
       </c>
       <c r="M36">
+        <v>53650</v>
+      </c>
+      <c r="N36">
         <v>24.88</v>
       </c>
     </row>
@@ -2055,7 +2192,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D37">
@@ -2079,10 +2216,16 @@
       <c r="J37">
         <v>0.120554396058822</v>
       </c>
+      <c r="K37">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L37">
         <v>0</v>
       </c>
       <c r="M37">
+        <v>55580</v>
+      </c>
+      <c r="N37">
         <v>6.03</v>
       </c>
     </row>
@@ -2099,7 +2242,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D38">
@@ -2130,6 +2273,9 @@
         <v>15583</v>
       </c>
       <c r="M38">
+        <v>57240</v>
+      </c>
+      <c r="N38">
         <v>17.16</v>
       </c>
     </row>
@@ -2146,7 +2292,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D39">
@@ -2170,10 +2316,16 @@
       <c r="J39">
         <v>0.2994430281898573</v>
       </c>
+      <c r="K39">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L39">
         <v>15484</v>
       </c>
       <c r="M39">
+        <v>54160</v>
+      </c>
+      <c r="N39">
         <v>37.19</v>
       </c>
     </row>
@@ -2190,7 +2342,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D40">
@@ -2214,10 +2366,16 @@
       <c r="J40">
         <v>0.1242853402984652</v>
       </c>
+      <c r="K40">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L40">
         <v>105592</v>
       </c>
       <c r="M40">
+        <v>53830</v>
+      </c>
+      <c r="N40">
         <v>34.62</v>
       </c>
     </row>
@@ -2234,7 +2392,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D41">
@@ -2265,6 +2423,9 @@
         <v>0</v>
       </c>
       <c r="M41">
+        <v>55790</v>
+      </c>
+      <c r="N41">
         <v>52.23</v>
       </c>
     </row>
@@ -2281,7 +2442,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D42">
@@ -2305,10 +2466,16 @@
       <c r="J42">
         <v>0.130676384825917</v>
       </c>
+      <c r="K42">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L42">
         <v>0</v>
       </c>
       <c r="M42">
+        <v>57720</v>
+      </c>
+      <c r="N42">
         <v>71.59999999999999</v>
       </c>
     </row>
@@ -2325,7 +2492,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D43">
@@ -2356,6 +2523,9 @@
         <v>0</v>
       </c>
       <c r="M43">
+        <v>53590</v>
+      </c>
+      <c r="N43">
         <v>76.41</v>
       </c>
     </row>
@@ -2372,7 +2542,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D44">
@@ -2403,6 +2573,9 @@
         <v>0</v>
       </c>
       <c r="M44">
+        <v>53780</v>
+      </c>
+      <c r="N44">
         <v>65.77</v>
       </c>
     </row>
@@ -2419,7 +2592,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D45">
@@ -2443,10 +2616,16 @@
       <c r="J45">
         <v>0.9417159190798167</v>
       </c>
+      <c r="K45">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L45">
         <v>29985</v>
       </c>
       <c r="M45">
+        <v>58000</v>
+      </c>
+      <c r="N45">
         <v>32.02</v>
       </c>
     </row>
@@ -2463,7 +2642,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D46">
@@ -2487,10 +2666,16 @@
       <c r="J46">
         <v>0.1746207155434114</v>
       </c>
+      <c r="K46">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L46">
         <v>20085</v>
       </c>
       <c r="M46">
+        <v>53570</v>
+      </c>
+      <c r="N46">
         <v>51.76</v>
       </c>
     </row>
@@ -2507,7 +2692,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D47">
@@ -2531,10 +2716,16 @@
       <c r="J47">
         <v>0.1342763104211891</v>
       </c>
+      <c r="K47">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L47">
         <v>20798</v>
       </c>
       <c r="M47">
+        <v>54860</v>
+      </c>
+      <c r="N47">
         <v>99.95</v>
       </c>
     </row>
@@ -2551,7 +2742,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D48">
@@ -2582,6 +2773,9 @@
         <v>0</v>
       </c>
       <c r="M48">
+        <v>57710</v>
+      </c>
+      <c r="N48">
         <v>81.22</v>
       </c>
     </row>
@@ -2598,7 +2792,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D49">
@@ -2622,10 +2816,16 @@
       <c r="J49">
         <v>0.3636450666718419</v>
       </c>
+      <c r="K49">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L49">
         <v>13654</v>
       </c>
       <c r="M49">
+        <v>55450</v>
+      </c>
+      <c r="N49">
         <v>26.78</v>
       </c>
     </row>
@@ -2642,7 +2842,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MC8re og Romsdal</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D50">
@@ -2673,6 +2873,9 @@
         <v>102285</v>
       </c>
       <c r="M50">
+        <v>51530</v>
+      </c>
+      <c r="N50">
         <v>76.48</v>
       </c>
     </row>
@@ -2689,7 +2892,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D51">
@@ -2713,10 +2916,16 @@
       <c r="J51">
         <v>0.3665115095323905</v>
       </c>
+      <c r="K51">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L51">
         <v>53918</v>
       </c>
       <c r="M51">
+        <v>54120</v>
+      </c>
+      <c r="N51">
         <v>47.24</v>
       </c>
     </row>
@@ -2733,7 +2942,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MØRE OG ROMSDAL</t>
+          <t>Møre og Romsdal</t>
         </is>
       </c>
       <c r="D52">
@@ -2757,10 +2966,16 @@
       <c r="J52">
         <v>0.1626791499749644</v>
       </c>
+      <c r="K52">
+        <v>8.921212499999999</v>
+      </c>
       <c r="L52">
         <v>0</v>
       </c>
       <c r="M52">
+        <v>54770</v>
+      </c>
+      <c r="N52">
         <v>33.09</v>
       </c>
     </row>
@@ -2808,6 +3023,9 @@
         <v>581309</v>
       </c>
       <c r="M53">
+        <v>58440</v>
+      </c>
+      <c r="N53">
         <v>8.050000000000001</v>
       </c>
     </row>
@@ -2855,6 +3073,9 @@
         <v>210944</v>
       </c>
       <c r="M54">
+        <v>55930</v>
+      </c>
+      <c r="N54">
         <v>15.42</v>
       </c>
     </row>
@@ -2902,6 +3123,9 @@
         <v>0</v>
       </c>
       <c r="M55">
+        <v>52450</v>
+      </c>
+      <c r="N55">
         <v>62.33</v>
       </c>
     </row>
@@ -2949,6 +3173,9 @@
         <v>0</v>
       </c>
       <c r="M56">
+        <v>53310</v>
+      </c>
+      <c r="N56">
         <v>52.02</v>
       </c>
     </row>
@@ -2996,6 +3223,9 @@
         <v>30622</v>
       </c>
       <c r="M57">
+        <v>54840</v>
+      </c>
+      <c r="N57">
         <v>27.55</v>
       </c>
     </row>
@@ -3043,6 +3273,9 @@
         <v>8237</v>
       </c>
       <c r="M58">
+        <v>53350</v>
+      </c>
+      <c r="N58">
         <v>74.59</v>
       </c>
     </row>
@@ -3090,6 +3323,9 @@
         <v>0</v>
       </c>
       <c r="M59">
+        <v>54710</v>
+      </c>
+      <c r="N59">
         <v>100</v>
       </c>
     </row>
@@ -3137,6 +3373,9 @@
         <v>4405</v>
       </c>
       <c r="M60">
+        <v>54650</v>
+      </c>
+      <c r="N60">
         <v>53.15</v>
       </c>
     </row>
@@ -3184,6 +3423,9 @@
         <v>26113</v>
       </c>
       <c r="M61">
+        <v>55170</v>
+      </c>
+      <c r="N61">
         <v>18.31</v>
       </c>
     </row>
@@ -3231,6 +3473,9 @@
         <v>0</v>
       </c>
       <c r="M62">
+        <v>53140</v>
+      </c>
+      <c r="N62">
         <v>67.05</v>
       </c>
     </row>
@@ -3278,6 +3523,9 @@
         <v>31160</v>
       </c>
       <c r="M63">
+        <v>54870</v>
+      </c>
+      <c r="N63">
         <v>25.27</v>
       </c>
     </row>
@@ -3325,6 +3573,9 @@
         <v>10406</v>
       </c>
       <c r="M64">
+        <v>50170</v>
+      </c>
+      <c r="N64">
         <v>40.57</v>
       </c>
     </row>
@@ -3372,6 +3623,9 @@
         <v>0</v>
       </c>
       <c r="M65">
+        <v>49190</v>
+      </c>
+      <c r="N65">
         <v>57.79</v>
       </c>
     </row>
@@ -3419,6 +3673,9 @@
         <v>3015</v>
       </c>
       <c r="M66">
+        <v>55160</v>
+      </c>
+      <c r="N66">
         <v>81.08</v>
       </c>
     </row>
@@ -3466,6 +3723,9 @@
         <v>0</v>
       </c>
       <c r="M67">
+        <v>53670</v>
+      </c>
+      <c r="N67">
         <v>23.17</v>
       </c>
     </row>
@@ -3513,6 +3773,9 @@
         <v>0</v>
       </c>
       <c r="M68">
+        <v>53740</v>
+      </c>
+      <c r="N68">
         <v>39.24</v>
       </c>
     </row>
@@ -3560,6 +3823,9 @@
         <v>166181</v>
       </c>
       <c r="M69">
+        <v>55660</v>
+      </c>
+      <c r="N69">
         <v>16.6</v>
       </c>
     </row>
@@ -3607,6 +3873,9 @@
         <v>0</v>
       </c>
       <c r="M70">
+        <v>57180</v>
+      </c>
+      <c r="N70">
         <v>72.16</v>
       </c>
     </row>
@@ -3654,6 +3923,9 @@
         <v>0</v>
       </c>
       <c r="M71">
+        <v>50870</v>
+      </c>
+      <c r="N71">
         <v>12.67</v>
       </c>
     </row>
@@ -3701,6 +3973,9 @@
         <v>0</v>
       </c>
       <c r="M72">
+        <v>55720</v>
+      </c>
+      <c r="N72">
         <v>100</v>
       </c>
     </row>
@@ -3748,6 +4023,9 @@
         <v>33851</v>
       </c>
       <c r="M73">
+        <v>55570</v>
+      </c>
+      <c r="N73">
         <v>42.33</v>
       </c>
     </row>
@@ -3795,6 +4073,9 @@
         <v>10679</v>
       </c>
       <c r="M74">
+        <v>53430</v>
+      </c>
+      <c r="N74">
         <v>67.56999999999999</v>
       </c>
     </row>
@@ -3842,6 +4123,9 @@
         <v>0</v>
       </c>
       <c r="M75">
+        <v>51370</v>
+      </c>
+      <c r="N75">
         <v>99.91</v>
       </c>
     </row>
@@ -3889,6 +4173,9 @@
         <v>31832</v>
       </c>
       <c r="M76">
+        <v>54350</v>
+      </c>
+      <c r="N76">
         <v>33.42</v>
       </c>
     </row>
@@ -3936,6 +4223,9 @@
         <v>34390</v>
       </c>
       <c r="M77">
+        <v>54740</v>
+      </c>
+      <c r="N77">
         <v>24.69</v>
       </c>
     </row>
@@ -3983,6 +4273,9 @@
         <v>0</v>
       </c>
       <c r="M78">
+        <v>53790</v>
+      </c>
+      <c r="N78">
         <v>53.88</v>
       </c>
     </row>
@@ -4030,6 +4323,9 @@
         <v>17742</v>
       </c>
       <c r="M79">
+        <v>55810</v>
+      </c>
+      <c r="N79">
         <v>90.83</v>
       </c>
     </row>
@@ -4077,6 +4373,9 @@
         <v>0</v>
       </c>
       <c r="M80">
+        <v>52330</v>
+      </c>
+      <c r="N80">
         <v>17.38</v>
       </c>
     </row>
@@ -4124,6 +4423,9 @@
         <v>5117</v>
       </c>
       <c r="M81">
+        <v>53360</v>
+      </c>
+      <c r="N81">
         <v>48.57</v>
       </c>
     </row>
@@ -4171,6 +4473,9 @@
         <v>0</v>
       </c>
       <c r="M82">
+        <v>50230</v>
+      </c>
+      <c r="N82">
         <v>30.22</v>
       </c>
     </row>
@@ -4218,6 +4523,9 @@
         <v>0</v>
       </c>
       <c r="M83">
+        <v>50970</v>
+      </c>
+      <c r="N83">
         <v>12.45</v>
       </c>
     </row>
@@ -4265,6 +4573,9 @@
         <v>26138</v>
       </c>
       <c r="M84">
+        <v>51570</v>
+      </c>
+      <c r="N84">
         <v>99.84</v>
       </c>
     </row>
@@ -4312,6 +4623,9 @@
         <v>92343</v>
       </c>
       <c r="M85">
+        <v>53040</v>
+      </c>
+      <c r="N85">
         <v>36.08</v>
       </c>
     </row>
@@ -4359,6 +4673,9 @@
         <v>441299</v>
       </c>
       <c r="M86">
+        <v>52810</v>
+      </c>
+      <c r="N86">
         <v>22.4</v>
       </c>
     </row>
@@ -4406,6 +4723,9 @@
         <v>55407</v>
       </c>
       <c r="M87">
+        <v>54300</v>
+      </c>
+      <c r="N87">
         <v>24.62</v>
       </c>
     </row>
@@ -4453,6 +4773,9 @@
         <v>24161</v>
       </c>
       <c r="M88">
+        <v>52530</v>
+      </c>
+      <c r="N88">
         <v>64.81</v>
       </c>
     </row>
@@ -4500,6 +4823,9 @@
         <v>0</v>
       </c>
       <c r="M89">
+        <v>52470</v>
+      </c>
+      <c r="N89">
         <v>44.25</v>
       </c>
     </row>
@@ -4547,6 +4873,9 @@
         <v>75509</v>
       </c>
       <c r="M90">
+        <v>54470</v>
+      </c>
+      <c r="N90">
         <v>31.37</v>
       </c>
     </row>
@@ -4594,6 +4923,9 @@
         <v>94508</v>
       </c>
       <c r="M91">
+        <v>54180</v>
+      </c>
+      <c r="N91">
         <v>35.14</v>
       </c>
     </row>
@@ -4641,6 +4973,9 @@
         <v>138321</v>
       </c>
       <c r="M92">
+        <v>48910</v>
+      </c>
+      <c r="N92">
         <v>27.46</v>
       </c>
     </row>
@@ -4688,6 +5023,9 @@
         <v>34894</v>
       </c>
       <c r="M93">
+        <v>55490</v>
+      </c>
+      <c r="N93">
         <v>68.05</v>
       </c>
     </row>
@@ -4704,7 +5042,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D94">
@@ -4728,10 +5066,16 @@
       <c r="J94">
         <v>0.2442896293388739</v>
       </c>
+      <c r="K94">
+        <v>203.3475</v>
+      </c>
       <c r="L94">
         <v>86004</v>
       </c>
       <c r="M94">
+        <v>55470</v>
+      </c>
+      <c r="N94">
         <v>12.55</v>
       </c>
     </row>
@@ -4748,7 +5092,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D95">
@@ -4772,10 +5116,16 @@
       <c r="J95">
         <v>0.4179704058803027</v>
       </c>
+      <c r="K95">
+        <v>203.3475</v>
+      </c>
       <c r="L95">
         <v>57442</v>
       </c>
       <c r="M95">
+        <v>58280</v>
+      </c>
+      <c r="N95">
         <v>3.69</v>
       </c>
     </row>
@@ -4792,7 +5142,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D96">
@@ -4816,10 +5166,16 @@
       <c r="J96">
         <v>0.363065088781134</v>
       </c>
+      <c r="K96">
+        <v>203.3475</v>
+      </c>
       <c r="L96">
         <v>0</v>
       </c>
       <c r="M96">
+        <v>54260</v>
+      </c>
+      <c r="N96">
         <v>8.789999999999999</v>
       </c>
     </row>
@@ -4836,7 +5192,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D97">
@@ -4860,10 +5216,16 @@
       <c r="J97">
         <v>0.7875826270011952</v>
       </c>
+      <c r="K97">
+        <v>203.3475</v>
+      </c>
       <c r="L97">
         <v>47847</v>
       </c>
       <c r="M97">
+        <v>56710</v>
+      </c>
+      <c r="N97">
         <v>6.31</v>
       </c>
     </row>
@@ -4880,7 +5242,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D98">
@@ -4904,10 +5266,16 @@
       <c r="J98">
         <v>0.1880250164650877</v>
       </c>
+      <c r="K98">
+        <v>203.3475</v>
+      </c>
       <c r="L98">
         <v>0</v>
       </c>
       <c r="M98">
+        <v>59290</v>
+      </c>
+      <c r="N98">
         <v>37.33</v>
       </c>
     </row>
@@ -4924,7 +5292,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>C_x0018_stfold</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D99">
@@ -4948,10 +5316,16 @@
       <c r="J99">
         <v>12.8910270925836</v>
       </c>
+      <c r="K99">
+        <v>203.3475</v>
+      </c>
       <c r="L99">
         <v>55235</v>
       </c>
       <c r="M99">
+        <v>55790</v>
+      </c>
+      <c r="N99">
         <v>22.17</v>
       </c>
     </row>
@@ -4968,7 +5342,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>C_x0018_stfold</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D100">
@@ -4992,10 +5366,16 @@
       <c r="J100">
         <v>10.7889312979334</v>
       </c>
+      <c r="K100">
+        <v>203.3475</v>
+      </c>
       <c r="L100">
         <v>0</v>
       </c>
       <c r="M100">
+        <v>55650</v>
+      </c>
+      <c r="N100">
         <v>30.95</v>
       </c>
     </row>
@@ -5012,7 +5392,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>C_x0018_stfold</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D101">
@@ -5036,10 +5416,16 @@
       <c r="J101">
         <v>11.51837921725955</v>
       </c>
+      <c r="K101">
+        <v>203.3475</v>
+      </c>
       <c r="L101">
         <v>0</v>
       </c>
       <c r="M101">
+        <v>53250</v>
+      </c>
+      <c r="N101">
         <v>50.19</v>
       </c>
     </row>
@@ -5056,7 +5442,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D102">
@@ -5080,10 +5466,16 @@
       <c r="J102">
         <v>0.5653232738183865</v>
       </c>
+      <c r="K102">
+        <v>203.3475</v>
+      </c>
       <c r="L102">
         <v>6053</v>
       </c>
       <c r="M102">
+        <v>53520</v>
+      </c>
+      <c r="N102">
         <v>21.43</v>
       </c>
     </row>
@@ -5100,7 +5492,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>ØSTFOLD</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D103">
@@ -5124,10 +5516,16 @@
       <c r="J103">
         <v>0.2023578968498255</v>
       </c>
+      <c r="K103">
+        <v>203.3475</v>
+      </c>
       <c r="L103">
         <v>0</v>
       </c>
       <c r="M103">
+        <v>52480</v>
+      </c>
+      <c r="N103">
         <v>36.76</v>
       </c>
     </row>
@@ -5144,7 +5542,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>C_x0018_stfold</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D104">
@@ -5168,10 +5566,16 @@
       <c r="J104">
         <v>18.95264226153718</v>
       </c>
+      <c r="K104">
+        <v>203.3475</v>
+      </c>
       <c r="L104">
         <v>0</v>
       </c>
       <c r="M104">
+        <v>53220</v>
+      </c>
+      <c r="N104">
         <v>49.15</v>
       </c>
     </row>
@@ -5188,7 +5592,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>C_x0018_stfold</t>
+          <t>Østfold</t>
         </is>
       </c>
       <c r="D105">
@@ -5212,10 +5616,16 @@
       <c r="J105">
         <v>21.04270846108081</v>
       </c>
+      <c r="K105">
+        <v>203.3475</v>
+      </c>
       <c r="L105">
         <v>0</v>
       </c>
       <c r="M105">
+        <v>52180</v>
+      </c>
+      <c r="N105">
         <v>99.93000000000001</v>
       </c>
     </row>
@@ -5263,6 +5673,9 @@
         <v>345089</v>
       </c>
       <c r="M106">
+        <v>76170</v>
+      </c>
+      <c r="N106">
         <v>0.95</v>
       </c>
     </row>
@@ -5310,6 +5723,9 @@
         <v>198740</v>
       </c>
       <c r="M107">
+        <v>69150</v>
+      </c>
+      <c r="N107">
         <v>5.04</v>
       </c>
     </row>
@@ -5357,6 +5773,9 @@
         <v>269120</v>
       </c>
       <c r="M108">
+        <v>59910</v>
+      </c>
+      <c r="N108">
         <v>6.88</v>
       </c>
     </row>
@@ -5404,6 +5823,9 @@
         <v>105100</v>
       </c>
       <c r="M109">
+        <v>65160</v>
+      </c>
+      <c r="N109">
         <v>5.5</v>
       </c>
     </row>
@@ -5451,6 +5873,9 @@
         <v>1188458</v>
       </c>
       <c r="M110">
+        <v>56350</v>
+      </c>
+      <c r="N110">
         <v>7.79</v>
       </c>
     </row>
@@ -5498,6 +5923,9 @@
         <v>0</v>
       </c>
       <c r="M111">
+        <v>65170</v>
+      </c>
+      <c r="N111">
         <v>9.24</v>
       </c>
     </row>
@@ -5545,6 +5973,9 @@
         <v>0</v>
       </c>
       <c r="M112">
+        <v>65260</v>
+      </c>
+      <c r="N112">
         <v>15.16</v>
       </c>
     </row>
@@ -5592,6 +6023,9 @@
         <v>0</v>
       </c>
       <c r="M113">
+        <v>60460</v>
+      </c>
+      <c r="N113">
         <v>14.79</v>
       </c>
     </row>
@@ -5639,6 +6073,9 @@
         <v>0</v>
       </c>
       <c r="M114">
+        <v>60530</v>
+      </c>
+      <c r="N114">
         <v>13.92</v>
       </c>
     </row>
@@ -5686,6 +6123,9 @@
         <v>0</v>
       </c>
       <c r="M115">
+        <v>55610</v>
+      </c>
+      <c r="N115">
         <v>19.86</v>
       </c>
     </row>
@@ -5733,6 +6173,9 @@
         <v>0</v>
       </c>
       <c r="M116">
+        <v>60400</v>
+      </c>
+      <c r="N116">
         <v>0.59</v>
       </c>
     </row>
@@ -5780,6 +6223,9 @@
         <v>0</v>
       </c>
       <c r="M117">
+        <v>60090</v>
+      </c>
+      <c r="N117">
         <v>2.83</v>
       </c>
     </row>
@@ -5827,6 +6273,9 @@
         <v>0</v>
       </c>
       <c r="M118">
+        <v>53650</v>
+      </c>
+      <c r="N118">
         <v>39.24</v>
       </c>
     </row>
@@ -5874,6 +6323,9 @@
         <v>14080</v>
       </c>
       <c r="M119">
+        <v>54820</v>
+      </c>
+      <c r="N119">
         <v>29.8</v>
       </c>
     </row>
@@ -5921,6 +6373,9 @@
         <v>0</v>
       </c>
       <c r="M120">
+        <v>61000</v>
+      </c>
+      <c r="N120">
         <v>23.61</v>
       </c>
     </row>
@@ -5968,6 +6423,9 @@
         <v>0</v>
       </c>
       <c r="M121">
+        <v>62260</v>
+      </c>
+      <c r="N121">
         <v>5.93</v>
       </c>
     </row>
@@ -6015,6 +6473,9 @@
         <v>0</v>
       </c>
       <c r="M122">
+        <v>56180</v>
+      </c>
+      <c r="N122">
         <v>34.99</v>
       </c>
     </row>
@@ -6062,6 +6523,9 @@
         <v>0</v>
       </c>
       <c r="M123">
+        <v>53850</v>
+      </c>
+      <c r="N123">
         <v>25.52</v>
       </c>
     </row>
@@ -6109,6 +6573,9 @@
         <v>0</v>
       </c>
       <c r="M124">
+        <v>54330</v>
+      </c>
+      <c r="N124">
         <v>20.13</v>
       </c>
     </row>
@@ -6156,6 +6623,9 @@
         <v>0</v>
       </c>
       <c r="M125">
+        <v>55310</v>
+      </c>
+      <c r="N125">
         <v>16.97</v>
       </c>
     </row>
@@ -6203,6 +6673,9 @@
         <v>0</v>
       </c>
       <c r="M126">
+        <v>54120</v>
+      </c>
+      <c r="N126">
         <v>61.39</v>
       </c>
     </row>
@@ -6250,6 +6723,9 @@
         <v>39925</v>
       </c>
       <c r="M127">
+        <v>57890</v>
+      </c>
+      <c r="N127">
         <v>2.22</v>
       </c>
     </row>
@@ -6297,6 +6773,9 @@
         <v>74917</v>
       </c>
       <c r="M128">
+        <v>61950</v>
+      </c>
+      <c r="N128">
         <v>12.96</v>
       </c>
     </row>
@@ -6344,6 +6823,9 @@
         <v>68591</v>
       </c>
       <c r="M129">
+        <v>54350</v>
+      </c>
+      <c r="N129">
         <v>25.94</v>
       </c>
     </row>
@@ -6391,6 +6873,9 @@
         <v>42801</v>
       </c>
       <c r="M130">
+        <v>63090</v>
+      </c>
+      <c r="N130">
         <v>34.9</v>
       </c>
     </row>
@@ -6438,6 +6923,9 @@
         <v>0</v>
       </c>
       <c r="M131">
+        <v>62170</v>
+      </c>
+      <c r="N131">
         <v>14.25</v>
       </c>
     </row>
@@ -6485,6 +6973,9 @@
         <v>0</v>
       </c>
       <c r="M132">
+        <v>55870</v>
+      </c>
+      <c r="N132">
         <v>17.6</v>
       </c>
     </row>
@@ -6532,6 +7023,9 @@
         <v>0</v>
       </c>
       <c r="M133">
+        <v>53460</v>
+      </c>
+      <c r="N133">
         <v>28.21</v>
       </c>
     </row>
@@ -6579,6 +7073,9 @@
         <v>0</v>
       </c>
       <c r="M134">
+        <v>52680</v>
+      </c>
+      <c r="N134">
         <v>57.03</v>
       </c>
     </row>
@@ -6626,6 +7123,9 @@
         <v>0</v>
       </c>
       <c r="M135">
+        <v>51400</v>
+      </c>
+      <c r="N135">
         <v>100</v>
       </c>
     </row>
@@ -6673,6 +7173,9 @@
         <v>11478</v>
       </c>
       <c r="M136">
+        <v>52460</v>
+      </c>
+      <c r="N136">
         <v>35.02</v>
       </c>
     </row>
@@ -6720,6 +7223,9 @@
         <v>249121</v>
       </c>
       <c r="M137">
+        <v>51770</v>
+      </c>
+      <c r="N137">
         <v>32.83</v>
       </c>
     </row>
@@ -6767,6 +7273,9 @@
         <v>280203</v>
       </c>
       <c r="M138">
+        <v>54330</v>
+      </c>
+      <c r="N138">
         <v>39.27</v>
       </c>
     </row>
@@ -6814,6 +7323,9 @@
         <v>46767</v>
       </c>
       <c r="M139">
+        <v>53180</v>
+      </c>
+      <c r="N139">
         <v>39.6</v>
       </c>
     </row>
@@ -6861,6 +7373,9 @@
         <v>424432</v>
       </c>
       <c r="M140">
+        <v>52120</v>
+      </c>
+      <c r="N140">
         <v>35.88</v>
       </c>
     </row>
@@ -6908,6 +7423,9 @@
         <v>16265</v>
       </c>
       <c r="M141">
+        <v>51990</v>
+      </c>
+      <c r="N141">
         <v>85.2</v>
       </c>
     </row>
@@ -6955,6 +7473,9 @@
         <v>0</v>
       </c>
       <c r="M142">
+        <v>54310</v>
+      </c>
+      <c r="N142">
         <v>63.61</v>
       </c>
     </row>
@@ -7002,6 +7523,9 @@
         <v>0</v>
       </c>
       <c r="M143">
+        <v>50890</v>
+      </c>
+      <c r="N143">
         <v>73.98</v>
       </c>
     </row>
@@ -7049,6 +7573,9 @@
         <v>44137</v>
       </c>
       <c r="M144">
+        <v>51010</v>
+      </c>
+      <c r="N144">
         <v>79.69</v>
       </c>
     </row>
@@ -7096,6 +7623,9 @@
         <v>28103</v>
       </c>
       <c r="M145">
+        <v>54520</v>
+      </c>
+      <c r="N145">
         <v>25.48</v>
       </c>
     </row>
@@ -7143,6 +7673,9 @@
         <v>195164</v>
       </c>
       <c r="M146">
+        <v>59110</v>
+      </c>
+      <c r="N146">
         <v>10.96</v>
       </c>
     </row>
@@ -7190,6 +7723,9 @@
         <v>484011</v>
       </c>
       <c r="M147">
+        <v>58200</v>
+      </c>
+      <c r="N147">
         <v>12.71</v>
       </c>
     </row>
@@ -7237,6 +7773,9 @@
         <v>152223</v>
       </c>
       <c r="M148">
+        <v>55960</v>
+      </c>
+      <c r="N148">
         <v>21.77</v>
       </c>
     </row>
@@ -7284,6 +7823,9 @@
         <v>111736</v>
       </c>
       <c r="M149">
+        <v>53530</v>
+      </c>
+      <c r="N149">
         <v>42.13</v>
       </c>
     </row>
@@ -7331,6 +7873,9 @@
         <v>0</v>
       </c>
       <c r="M150">
+        <v>51980</v>
+      </c>
+      <c r="N150">
         <v>40.21</v>
       </c>
     </row>
@@ -7378,6 +7923,9 @@
         <v>0</v>
       </c>
       <c r="M151">
+        <v>55300</v>
+      </c>
+      <c r="N151">
         <v>34.86</v>
       </c>
     </row>
@@ -7425,6 +7973,9 @@
         <v>0</v>
       </c>
       <c r="M152">
+        <v>51920</v>
+      </c>
+      <c r="N152">
         <v>68.98999999999999</v>
       </c>
     </row>
@@ -7472,6 +8023,9 @@
         <v>0</v>
       </c>
       <c r="M153">
+        <v>53430</v>
+      </c>
+      <c r="N153">
         <v>59.52</v>
       </c>
     </row>
@@ -7519,6 +8073,9 @@
         <v>0</v>
       </c>
       <c r="M154">
+        <v>51240</v>
+      </c>
+      <c r="N154">
         <v>61.27</v>
       </c>
     </row>
@@ -7566,6 +8123,9 @@
         <v>4301</v>
       </c>
       <c r="M155">
+        <v>50940</v>
+      </c>
+      <c r="N155">
         <v>72.93000000000001</v>
       </c>
     </row>
@@ -7613,6 +8173,9 @@
         <v>0</v>
       </c>
       <c r="M156">
+        <v>51100</v>
+      </c>
+      <c r="N156">
         <v>69.66</v>
       </c>
     </row>
@@ -7660,6 +8223,9 @@
         <v>0</v>
       </c>
       <c r="M157">
+        <v>49650</v>
+      </c>
+      <c r="N157">
         <v>62.41</v>
       </c>
     </row>
@@ -7707,6 +8273,9 @@
         <v>0</v>
       </c>
       <c r="M158">
+        <v>55300</v>
+      </c>
+      <c r="N158">
         <v>24.76</v>
       </c>
     </row>
@@ -7754,6 +8323,9 @@
         <v>62906</v>
       </c>
       <c r="M159">
+        <v>50440</v>
+      </c>
+      <c r="N159">
         <v>55.25</v>
       </c>
     </row>
@@ -7801,6 +8373,9 @@
         <v>8870</v>
       </c>
       <c r="M160">
+        <v>55570</v>
+      </c>
+      <c r="N160">
         <v>50.62</v>
       </c>
     </row>
@@ -7848,6 +8423,9 @@
         <v>19284</v>
       </c>
       <c r="M161">
+        <v>50260</v>
+      </c>
+      <c r="N161">
         <v>55.54</v>
       </c>
     </row>
@@ -7895,6 +8473,9 @@
         <v>0</v>
       </c>
       <c r="M162">
+        <v>49220</v>
+      </c>
+      <c r="N162">
         <v>85.3</v>
       </c>
     </row>
@@ -7942,6 +8523,9 @@
         <v>44363</v>
       </c>
       <c r="M163">
+        <v>48880</v>
+      </c>
+      <c r="N163">
         <v>77.44</v>
       </c>
     </row>
@@ -7989,6 +8573,9 @@
         <v>0</v>
       </c>
       <c r="M164">
+        <v>51730</v>
+      </c>
+      <c r="N164">
         <v>60.85</v>
       </c>
     </row>
@@ -8036,6 +8623,9 @@
         <v>0</v>
       </c>
       <c r="M165">
+        <v>51800</v>
+      </c>
+      <c r="N165">
         <v>47.7</v>
       </c>
     </row>
@@ -8083,6 +8673,9 @@
         <v>7210</v>
       </c>
       <c r="M166">
+        <v>51420</v>
+      </c>
+      <c r="N166">
         <v>66.15000000000001</v>
       </c>
     </row>
@@ -8130,6 +8723,9 @@
         <v>18351</v>
       </c>
       <c r="M167">
+        <v>51440</v>
+      </c>
+      <c r="N167">
         <v>66.78</v>
       </c>
     </row>
@@ -8177,6 +8773,9 @@
         <v>0</v>
       </c>
       <c r="M168">
+        <v>51120</v>
+      </c>
+      <c r="N168">
         <v>63.62</v>
       </c>
     </row>
@@ -8224,6 +8823,9 @@
         <v>127348</v>
       </c>
       <c r="M169">
+        <v>51180</v>
+      </c>
+      <c r="N169">
         <v>53.5</v>
       </c>
     </row>
@@ -8271,6 +8873,9 @@
         <v>12482</v>
       </c>
       <c r="M170">
+        <v>51430</v>
+      </c>
+      <c r="N170">
         <v>88.34999999999999</v>
       </c>
     </row>
@@ -8318,6 +8923,9 @@
         <v>53401</v>
       </c>
       <c r="M171">
+        <v>50260</v>
+      </c>
+      <c r="N171">
         <v>70.53</v>
       </c>
     </row>
@@ -8365,6 +8973,9 @@
         <v>178017</v>
       </c>
       <c r="M172">
+        <v>51350</v>
+      </c>
+      <c r="N172">
         <v>62.07</v>
       </c>
     </row>
@@ -8412,6 +9023,9 @@
         <v>127798</v>
       </c>
       <c r="M173">
+        <v>52070</v>
+      </c>
+      <c r="N173">
         <v>49.05</v>
       </c>
     </row>
@@ -8459,6 +9073,9 @@
         <v>46751</v>
       </c>
       <c r="M174">
+        <v>54390</v>
+      </c>
+      <c r="N174">
         <v>38.67</v>
       </c>
     </row>
@@ -8506,6 +9123,9 @@
         <v>120682</v>
       </c>
       <c r="M175">
+        <v>51780</v>
+      </c>
+      <c r="N175">
         <v>49.03</v>
       </c>
     </row>
@@ -8553,6 +9173,9 @@
         <v>71305</v>
       </c>
       <c r="M176">
+        <v>52640</v>
+      </c>
+      <c r="N176">
         <v>62.46</v>
       </c>
     </row>
@@ -8600,6 +9223,9 @@
         <v>114666</v>
       </c>
       <c r="M177">
+        <v>50730</v>
+      </c>
+      <c r="N177">
         <v>51.89</v>
       </c>
     </row>
@@ -8647,6 +9273,9 @@
         <v>210399</v>
       </c>
       <c r="M178">
+        <v>52960</v>
+      </c>
+      <c r="N178">
         <v>40.22</v>
       </c>
     </row>
@@ -8694,6 +9323,9 @@
         <v>75962</v>
       </c>
       <c r="M179">
+        <v>51680</v>
+      </c>
+      <c r="N179">
         <v>52.78</v>
       </c>
     </row>
@@ -8741,6 +9373,9 @@
         <v>0</v>
       </c>
       <c r="M180">
+        <v>53310</v>
+      </c>
+      <c r="N180">
         <v>52.28</v>
       </c>
     </row>
@@ -8788,6 +9423,9 @@
         <v>0</v>
       </c>
       <c r="M181">
+        <v>53310</v>
+      </c>
+      <c r="N181">
         <v>24.58</v>
       </c>
     </row>
@@ -8835,6 +9473,9 @@
         <v>32758</v>
       </c>
       <c r="M182">
+        <v>54540</v>
+      </c>
+      <c r="N182">
         <v>49.61</v>
       </c>
     </row>
@@ -8882,6 +9523,9 @@
         <v>0</v>
       </c>
       <c r="M183">
+        <v>52170</v>
+      </c>
+      <c r="N183">
         <v>61.79</v>
       </c>
     </row>
@@ -8929,6 +9573,9 @@
         <v>0</v>
       </c>
       <c r="M184">
+        <v>50900</v>
+      </c>
+      <c r="N184">
         <v>54.76</v>
       </c>
     </row>
@@ -8976,6 +9623,9 @@
         <v>0</v>
       </c>
       <c r="M185">
+        <v>51360</v>
+      </c>
+      <c r="N185">
         <v>78.28</v>
       </c>
     </row>
@@ -9023,6 +9673,9 @@
         <v>0</v>
       </c>
       <c r="M186">
+        <v>50650</v>
+      </c>
+      <c r="N186">
         <v>83.31</v>
       </c>
     </row>
@@ -9070,6 +9723,9 @@
         <v>275901</v>
       </c>
       <c r="M187">
+        <v>51220</v>
+      </c>
+      <c r="N187">
         <v>45.06</v>
       </c>
     </row>
@@ -9117,6 +9773,9 @@
         <v>0</v>
       </c>
       <c r="M188">
+        <v>50740</v>
+      </c>
+      <c r="N188">
         <v>72.34999999999999</v>
       </c>
     </row>
@@ -9164,6 +9823,9 @@
         <v>0</v>
       </c>
       <c r="M189">
+        <v>50900</v>
+      </c>
+      <c r="N189">
         <v>69.44</v>
       </c>
     </row>
@@ -9211,6 +9873,9 @@
         <v>29174</v>
       </c>
       <c r="M190">
+        <v>50410</v>
+      </c>
+      <c r="N190">
         <v>85.78</v>
       </c>
     </row>
@@ -9258,6 +9923,9 @@
         <v>99222</v>
       </c>
       <c r="M191">
+        <v>56870</v>
+      </c>
+      <c r="N191">
         <v>5.05</v>
       </c>
     </row>
@@ -9305,6 +9973,9 @@
         <v>26283</v>
       </c>
       <c r="M192">
+        <v>57150</v>
+      </c>
+      <c r="N192">
         <v>23.88</v>
       </c>
     </row>
@@ -9352,6 +10023,9 @@
         <v>126849</v>
       </c>
       <c r="M193">
+        <v>58410</v>
+      </c>
+      <c r="N193">
         <v>11.72</v>
       </c>
     </row>
@@ -9399,6 +10073,9 @@
         <v>475192</v>
       </c>
       <c r="M194">
+        <v>56530</v>
+      </c>
+      <c r="N194">
         <v>11.9</v>
       </c>
     </row>
@@ -9446,6 +10123,9 @@
         <v>533586</v>
       </c>
       <c r="M195">
+        <v>55710</v>
+      </c>
+      <c r="N195">
         <v>17.31</v>
       </c>
     </row>
@@ -9493,6 +10173,9 @@
         <v>49003</v>
       </c>
       <c r="M196">
+        <v>61360</v>
+      </c>
+      <c r="N196">
         <v>12.17</v>
       </c>
     </row>
@@ -9540,6 +10223,9 @@
         <v>0</v>
       </c>
       <c r="M197">
+        <v>59070</v>
+      </c>
+      <c r="N197">
         <v>4.16</v>
       </c>
     </row>
@@ -9587,6 +10273,9 @@
         <v>96805</v>
       </c>
       <c r="M198">
+        <v>56630</v>
+      </c>
+      <c r="N198">
         <v>8.91</v>
       </c>
     </row>
@@ -9634,6 +10323,9 @@
         <v>0</v>
       </c>
       <c r="M199">
+        <v>54600</v>
+      </c>
+      <c r="N199">
         <v>25.43</v>
       </c>
     </row>
@@ -9681,6 +10373,9 @@
         <v>0</v>
       </c>
       <c r="M200">
+        <v>55150</v>
+      </c>
+      <c r="N200">
         <v>35.05</v>
       </c>
     </row>
@@ -9728,6 +10423,9 @@
         <v>0</v>
       </c>
       <c r="M201">
+        <v>58110</v>
+      </c>
+      <c r="N201">
         <v>15.59</v>
       </c>
     </row>
@@ -9775,6 +10473,9 @@
         <v>126920</v>
       </c>
       <c r="M202">
+        <v>55020</v>
+      </c>
+      <c r="N202">
         <v>23.2</v>
       </c>
     </row>
@@ -9822,6 +10523,9 @@
         <v>0</v>
       </c>
       <c r="M203">
+        <v>54420</v>
+      </c>
+      <c r="N203">
         <v>59.54</v>
       </c>
     </row>
@@ -9869,6 +10573,9 @@
         <v>0</v>
       </c>
       <c r="M204">
+        <v>52880</v>
+      </c>
+      <c r="N204">
         <v>37.93</v>
       </c>
     </row>
@@ -9916,6 +10623,9 @@
         <v>0</v>
       </c>
       <c r="M205">
+        <v>53770</v>
+      </c>
+      <c r="N205">
         <v>44.76</v>
       </c>
     </row>
@@ -9963,6 +10673,9 @@
         <v>56905</v>
       </c>
       <c r="M206">
+        <v>55330</v>
+      </c>
+      <c r="N206">
         <v>50.05</v>
       </c>
     </row>
@@ -10010,6 +10723,9 @@
         <v>0</v>
       </c>
       <c r="M207">
+        <v>53150</v>
+      </c>
+      <c r="N207">
         <v>100</v>
       </c>
     </row>
@@ -10057,6 +10773,9 @@
         <v>163090</v>
       </c>
       <c r="M208">
+        <v>54870</v>
+      </c>
+      <c r="N208">
         <v>32.73</v>
       </c>
     </row>
@@ -10104,6 +10823,9 @@
         <v>21278</v>
       </c>
       <c r="M209">
+        <v>56320</v>
+      </c>
+      <c r="N209">
         <v>66.76000000000001</v>
       </c>
     </row>
@@ -10151,6 +10873,9 @@
         <v>14107</v>
       </c>
       <c r="M210">
+        <v>53640</v>
+      </c>
+      <c r="N210">
         <v>62.13</v>
       </c>
     </row>
@@ -10198,6 +10923,9 @@
         <v>0</v>
       </c>
       <c r="M211">
+        <v>53640</v>
+      </c>
+      <c r="N211">
         <v>70.14</v>
       </c>
     </row>
@@ -10245,6 +10973,9 @@
         <v>0</v>
       </c>
       <c r="M212">
+        <v>56590</v>
+      </c>
+      <c r="N212">
         <v>74.31999999999999</v>
       </c>
     </row>
@@ -10292,6 +11023,9 @@
         <v>117606</v>
       </c>
       <c r="M213">
+        <v>55150</v>
+      </c>
+      <c r="N213">
         <v>67.05</v>
       </c>
     </row>
@@ -10339,6 +11073,9 @@
         <v>52622</v>
       </c>
       <c r="M214">
+        <v>55260</v>
+      </c>
+      <c r="N214">
         <v>32.21</v>
       </c>
     </row>
@@ -10386,6 +11123,9 @@
         <v>108590</v>
       </c>
       <c r="M215">
+        <v>56000</v>
+      </c>
+      <c r="N215">
         <v>12.82</v>
       </c>
     </row>
@@ -10433,6 +11173,9 @@
         <v>98174</v>
       </c>
       <c r="M216">
+        <v>57440</v>
+      </c>
+      <c r="N216">
         <v>12.06</v>
       </c>
     </row>
@@ -10480,6 +11223,9 @@
         <v>136017</v>
       </c>
       <c r="M217">
+        <v>57550</v>
+      </c>
+      <c r="N217">
         <v>4.88</v>
       </c>
     </row>
@@ -10527,6 +11273,9 @@
         <v>164097</v>
       </c>
       <c r="M218">
+        <v>55570</v>
+      </c>
+      <c r="N218">
         <v>31.75</v>
       </c>
     </row>
@@ -10574,6 +11323,9 @@
         <v>32764</v>
       </c>
       <c r="M219">
+        <v>55290</v>
+      </c>
+      <c r="N219">
         <v>32.12</v>
       </c>
     </row>
@@ -10621,6 +11373,9 @@
         <v>0</v>
       </c>
       <c r="M220">
+        <v>56360</v>
+      </c>
+      <c r="N220">
         <v>26.55</v>
       </c>
     </row>
@@ -10668,6 +11423,9 @@
         <v>0</v>
       </c>
       <c r="M221">
+        <v>52250</v>
+      </c>
+      <c r="N221">
         <v>60.15</v>
       </c>
     </row>
@@ -10715,6 +11473,9 @@
         <v>0</v>
       </c>
       <c r="M222">
+        <v>54230</v>
+      </c>
+      <c r="N222">
         <v>57.85</v>
       </c>
     </row>
@@ -10762,6 +11523,9 @@
         <v>0</v>
       </c>
       <c r="M223">
+        <v>54760</v>
+      </c>
+      <c r="N223">
         <v>50.23</v>
       </c>
     </row>
@@ -10809,6 +11573,9 @@
         <v>0</v>
       </c>
       <c r="M224">
+        <v>53590</v>
+      </c>
+      <c r="N224">
         <v>45.43</v>
       </c>
     </row>
@@ -10856,6 +11623,9 @@
         <v>81604</v>
       </c>
       <c r="M225">
+        <v>57680</v>
+      </c>
+      <c r="N225">
         <v>24.17</v>
       </c>
     </row>
@@ -10903,6 +11673,9 @@
         <v>0</v>
       </c>
       <c r="M226">
+        <v>52840</v>
+      </c>
+      <c r="N226">
         <v>44.32</v>
       </c>
     </row>
@@ -10950,6 +11723,9 @@
         <v>0</v>
       </c>
       <c r="M227">
+        <v>53620</v>
+      </c>
+      <c r="N227">
         <v>60.93</v>
       </c>
     </row>
@@ -10997,6 +11773,9 @@
         <v>0</v>
       </c>
       <c r="M228">
+        <v>51880</v>
+      </c>
+      <c r="N228">
         <v>100</v>
       </c>
     </row>
@@ -11044,6 +11823,9 @@
         <v>77107</v>
       </c>
       <c r="M229">
+        <v>52280</v>
+      </c>
+      <c r="N229">
         <v>28.71</v>
       </c>
     </row>
@@ -11091,6 +11873,9 @@
         <v>0</v>
       </c>
       <c r="M230">
+        <v>52990</v>
+      </c>
+      <c r="N230">
         <v>48.9</v>
       </c>
     </row>
@@ -11138,6 +11923,9 @@
         <v>27190</v>
       </c>
       <c r="M231">
+        <v>54960</v>
+      </c>
+      <c r="N231">
         <v>99.92</v>
       </c>
     </row>
@@ -11185,6 +11973,9 @@
         <v>60455</v>
       </c>
       <c r="M232">
+        <v>52300</v>
+      </c>
+      <c r="N232">
         <v>33.04</v>
       </c>
     </row>
@@ -11232,6 +12023,9 @@
         <v>0</v>
       </c>
       <c r="M233">
+        <v>52880</v>
+      </c>
+      <c r="N233">
         <v>16.39</v>
       </c>
     </row>
@@ -11279,6 +12073,9 @@
         <v>0</v>
       </c>
       <c r="M234">
+        <v>54450</v>
+      </c>
+      <c r="N234">
         <v>100</v>
       </c>
     </row>
@@ -11326,6 +12123,9 @@
         <v>0</v>
       </c>
       <c r="M235">
+        <v>53180</v>
+      </c>
+      <c r="N235">
         <v>42.51</v>
       </c>
     </row>
@@ -11373,6 +12173,9 @@
         <v>0</v>
       </c>
       <c r="M236">
+        <v>54570</v>
+      </c>
+      <c r="N236">
         <v>86.59999999999999</v>
       </c>
     </row>
@@ -11420,6 +12223,9 @@
         <v>0</v>
       </c>
       <c r="M237">
+        <v>54590</v>
+      </c>
+      <c r="N237">
         <v>45.62</v>
       </c>
     </row>
@@ -11467,6 +12273,9 @@
         <v>46900</v>
       </c>
       <c r="M238">
+        <v>54920</v>
+      </c>
+      <c r="N238">
         <v>51.79</v>
       </c>
     </row>
@@ -11514,6 +12323,9 @@
         <v>2788040</v>
       </c>
       <c r="M239">
+        <v>61420</v>
+      </c>
+      <c r="N239">
         <v>1.92</v>
       </c>
     </row>
@@ -11561,6 +12373,9 @@
         <v>94159</v>
       </c>
       <c r="M240">
+        <v>56040</v>
+      </c>
+      <c r="N240">
         <v>16.42</v>
       </c>
     </row>
@@ -11608,6 +12423,9 @@
         <v>0</v>
       </c>
       <c r="M241">
+        <v>55250</v>
+      </c>
+      <c r="N241">
         <v>53.71</v>
       </c>
     </row>
@@ -11655,6 +12473,9 @@
         <v>11071</v>
       </c>
       <c r="M242">
+        <v>57020</v>
+      </c>
+      <c r="N242">
         <v>61.04</v>
       </c>
     </row>
@@ -11702,6 +12523,9 @@
         <v>0</v>
       </c>
       <c r="M243">
+        <v>58960</v>
+      </c>
+      <c r="N243">
         <v>38.36</v>
       </c>
     </row>
@@ -11749,6 +12573,9 @@
         <v>7810</v>
       </c>
       <c r="M244">
+        <v>58610</v>
+      </c>
+      <c r="N244">
         <v>5.48</v>
       </c>
     </row>
@@ -11796,6 +12623,9 @@
         <v>0</v>
       </c>
       <c r="M245">
+        <v>56370</v>
+      </c>
+      <c r="N245">
         <v>43.18</v>
       </c>
     </row>
@@ -11843,6 +12673,9 @@
         <v>7592</v>
       </c>
       <c r="M246">
+        <v>59490</v>
+      </c>
+      <c r="N246">
         <v>70.26000000000001</v>
       </c>
     </row>
@@ -11890,6 +12723,9 @@
         <v>0</v>
       </c>
       <c r="M247">
+        <v>56890</v>
+      </c>
+      <c r="N247">
         <v>34.8</v>
       </c>
     </row>
@@ -11937,6 +12773,9 @@
         <v>352251</v>
       </c>
       <c r="M248">
+        <v>55340</v>
+      </c>
+      <c r="N248">
         <v>30.83</v>
       </c>
     </row>
@@ -11984,6 +12823,9 @@
         <v>70757</v>
       </c>
       <c r="M249">
+        <v>55840</v>
+      </c>
+      <c r="N249">
         <v>40.7</v>
       </c>
     </row>
@@ -12031,6 +12873,9 @@
         <v>46571</v>
       </c>
       <c r="M250">
+        <v>53470</v>
+      </c>
+      <c r="N250">
         <v>51.24</v>
       </c>
     </row>
@@ -12078,6 +12923,9 @@
         <v>370144</v>
       </c>
       <c r="M251">
+        <v>54940</v>
+      </c>
+      <c r="N251">
         <v>37.03</v>
       </c>
     </row>
@@ -12125,6 +12973,9 @@
         <v>0</v>
       </c>
       <c r="M252">
+        <v>56990</v>
+      </c>
+      <c r="N252">
         <v>29.17</v>
       </c>
     </row>
@@ -12172,6 +13023,9 @@
         <v>0</v>
       </c>
       <c r="M253">
+        <v>56840</v>
+      </c>
+      <c r="N253">
         <v>57.59</v>
       </c>
     </row>
@@ -12219,6 +13073,9 @@
         <v>8728</v>
       </c>
       <c r="M254">
+        <v>58560</v>
+      </c>
+      <c r="N254">
         <v>22.79</v>
       </c>
     </row>
@@ -12266,6 +13123,9 @@
         <v>0</v>
       </c>
       <c r="M255">
+        <v>59370</v>
+      </c>
+      <c r="N255">
         <v>52.74</v>
       </c>
     </row>
@@ -12313,6 +13173,9 @@
         <v>19269</v>
       </c>
       <c r="M256">
+        <v>58580</v>
+      </c>
+      <c r="N256">
         <v>22.58</v>
       </c>
     </row>
@@ -12360,6 +13223,9 @@
         <v>0</v>
       </c>
       <c r="M257">
+        <v>58770</v>
+      </c>
+      <c r="N257">
         <v>9.09</v>
       </c>
     </row>
@@ -12407,6 +13273,9 @@
         <v>0</v>
       </c>
       <c r="M258">
+        <v>54950</v>
+      </c>
+      <c r="N258">
         <v>25.99</v>
       </c>
     </row>
@@ -12454,6 +13323,9 @@
         <v>0</v>
       </c>
       <c r="M259">
+        <v>53640</v>
+      </c>
+      <c r="N259">
         <v>99.73999999999999</v>
       </c>
     </row>
@@ -12501,6 +13373,9 @@
         <v>0</v>
       </c>
       <c r="M260">
+        <v>53920</v>
+      </c>
+      <c r="N260">
         <v>47.93</v>
       </c>
     </row>
@@ -12548,6 +13423,9 @@
         <v>25652</v>
       </c>
       <c r="M261">
+        <v>57710</v>
+      </c>
+      <c r="N261">
         <v>40.57</v>
       </c>
     </row>
@@ -12595,6 +13473,9 @@
         <v>0</v>
       </c>
       <c r="M262">
+        <v>58850</v>
+      </c>
+      <c r="N262">
         <v>62.17</v>
       </c>
     </row>
@@ -12642,6 +13523,9 @@
         <v>0</v>
       </c>
       <c r="M263">
+        <v>61200</v>
+      </c>
+      <c r="N263">
         <v>24.66</v>
       </c>
     </row>
@@ -12689,6 +13573,9 @@
         <v>0</v>
       </c>
       <c r="M264">
+        <v>55350</v>
+      </c>
+      <c r="N264">
         <v>100</v>
       </c>
     </row>
@@ -12736,6 +13623,9 @@
         <v>17626</v>
       </c>
       <c r="M265">
+        <v>54720</v>
+      </c>
+      <c r="N265">
         <v>71.84</v>
       </c>
     </row>
@@ -12783,6 +13673,9 @@
         <v>0</v>
       </c>
       <c r="M266">
+        <v>54650</v>
+      </c>
+      <c r="N266">
         <v>62.13</v>
       </c>
     </row>
@@ -12830,6 +13723,9 @@
         <v>4203</v>
       </c>
       <c r="M267">
+        <v>53530</v>
+      </c>
+      <c r="N267">
         <v>99.68000000000001</v>
       </c>
     </row>
@@ -12877,6 +13773,9 @@
         <v>0</v>
       </c>
       <c r="M268">
+        <v>55790</v>
+      </c>
+      <c r="N268">
         <v>36.04</v>
       </c>
     </row>
@@ -12924,6 +13823,9 @@
         <v>25193</v>
       </c>
       <c r="M269">
+        <v>53770</v>
+      </c>
+      <c r="N269">
         <v>52.06</v>
       </c>
     </row>
@@ -12971,6 +13873,9 @@
         <v>246632</v>
       </c>
       <c r="M270">
+        <v>54650</v>
+      </c>
+      <c r="N270">
         <v>23.13</v>
       </c>
     </row>
@@ -13018,6 +13923,9 @@
         <v>264919</v>
       </c>
       <c r="M271">
+        <v>52480</v>
+      </c>
+      <c r="N271">
         <v>39.17</v>
       </c>
     </row>
@@ -13065,6 +13973,9 @@
         <v>91891</v>
       </c>
       <c r="M272">
+        <v>53940</v>
+      </c>
+      <c r="N272">
         <v>45.56</v>
       </c>
     </row>
@@ -13112,6 +14023,9 @@
         <v>0</v>
       </c>
       <c r="M273">
+        <v>58990</v>
+      </c>
+      <c r="N273">
         <v>5.94</v>
       </c>
     </row>
@@ -13159,6 +14073,9 @@
         <v>142297</v>
       </c>
       <c r="M274">
+        <v>52630</v>
+      </c>
+      <c r="N274">
         <v>54.24</v>
       </c>
     </row>
@@ -13206,6 +14123,9 @@
         <v>3718</v>
       </c>
       <c r="M275">
+        <v>54690</v>
+      </c>
+      <c r="N275">
         <v>75.45</v>
       </c>
     </row>
@@ -13253,6 +14173,9 @@
         <v>0</v>
       </c>
       <c r="M276">
+        <v>55100</v>
+      </c>
+      <c r="N276">
         <v>47.3</v>
       </c>
     </row>
@@ -13300,6 +14223,9 @@
         <v>199489</v>
       </c>
       <c r="M277">
+        <v>55730</v>
+      </c>
+      <c r="N277">
         <v>30.98</v>
       </c>
     </row>
@@ -13347,6 +14273,9 @@
         <v>0</v>
       </c>
       <c r="M278">
+        <v>54370</v>
+      </c>
+      <c r="N278">
         <v>55.34</v>
       </c>
     </row>
@@ -13394,6 +14323,9 @@
         <v>0</v>
       </c>
       <c r="M279">
+        <v>53940</v>
+      </c>
+      <c r="N279">
         <v>45.93</v>
       </c>
     </row>
@@ -13441,6 +14373,9 @@
         <v>33133</v>
       </c>
       <c r="M280">
+        <v>53840</v>
+      </c>
+      <c r="N280">
         <v>50.37</v>
       </c>
     </row>
@@ -13488,6 +14423,9 @@
         <v>341705</v>
       </c>
       <c r="M281">
+        <v>51000</v>
+      </c>
+      <c r="N281">
         <v>46.24</v>
       </c>
     </row>
@@ -13504,7 +14442,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D282">
@@ -13528,10 +14466,16 @@
       <c r="J282">
         <v>0.2315682892224986</v>
       </c>
+      <c r="K282">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L282">
         <v>1278554</v>
       </c>
       <c r="M282">
+        <v>60880</v>
+      </c>
+      <c r="N282">
         <v>3</v>
       </c>
     </row>
@@ -13548,7 +14492,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D283">
@@ -13572,10 +14516,16 @@
       <c r="J283">
         <v>0.3563970951281953</v>
       </c>
+      <c r="K283">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L283">
         <v>26292</v>
       </c>
       <c r="M283">
+        <v>54010</v>
+      </c>
+      <c r="N283">
         <v>32.91</v>
       </c>
     </row>
@@ -13592,7 +14542,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D284">
@@ -13616,10 +14566,16 @@
       <c r="J284">
         <v>0.3812735850844319</v>
       </c>
+      <c r="K284">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L284">
         <v>24688</v>
       </c>
       <c r="M284">
+        <v>55400</v>
+      </c>
+      <c r="N284">
         <v>27.05</v>
       </c>
     </row>
@@ -13636,7 +14592,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D285">
@@ -13660,10 +14616,16 @@
       <c r="J285">
         <v>0.2316106446318464</v>
       </c>
+      <c r="K285">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L285">
         <v>0</v>
       </c>
       <c r="M285">
+        <v>54870</v>
+      </c>
+      <c r="N285">
         <v>66.53</v>
       </c>
     </row>
@@ -13680,7 +14642,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D286">
@@ -13704,10 +14666,16 @@
       <c r="J286">
         <v>40.16124405499531</v>
       </c>
+      <c r="K286">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L286">
         <v>0</v>
       </c>
       <c r="M286">
+        <v>51780</v>
+      </c>
+      <c r="N286">
         <v>99.89</v>
       </c>
     </row>
@@ -13724,7 +14692,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D287">
@@ -13748,10 +14716,16 @@
       <c r="J287">
         <v>0.1438713589994311</v>
       </c>
+      <c r="K287">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L287">
         <v>0</v>
       </c>
       <c r="M287">
+        <v>53330</v>
+      </c>
+      <c r="N287">
         <v>37.2</v>
       </c>
     </row>
@@ -13768,7 +14742,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D288">
@@ -13792,10 +14766,16 @@
       <c r="J288">
         <v>28.19494477479097</v>
       </c>
+      <c r="K288">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L288">
         <v>0</v>
       </c>
       <c r="M288">
+        <v>50190</v>
+      </c>
+      <c r="N288">
         <v>59.54</v>
       </c>
     </row>
@@ -13812,7 +14792,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D289">
@@ -13836,10 +14816,16 @@
       <c r="J289">
         <v>0.3432629468001519</v>
       </c>
+      <c r="K289">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L289">
         <v>0</v>
       </c>
       <c r="M289">
+        <v>52180</v>
+      </c>
+      <c r="N289">
         <v>31.19</v>
       </c>
     </row>
@@ -13856,7 +14842,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D290">
@@ -13880,10 +14866,16 @@
       <c r="J290">
         <v>30.12950947722824</v>
       </c>
+      <c r="K290">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L290">
         <v>0</v>
       </c>
       <c r="M290">
+        <v>52490</v>
+      </c>
+      <c r="N290">
         <v>69.29000000000001</v>
       </c>
     </row>
@@ -13900,7 +14892,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D291">
@@ -13924,10 +14916,16 @@
       <c r="J291">
         <v>1.296233999884783</v>
       </c>
+      <c r="K291">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L291">
         <v>0</v>
       </c>
       <c r="M291">
+        <v>52010</v>
+      </c>
+      <c r="N291">
         <v>57.43</v>
       </c>
     </row>
@@ -13944,7 +14942,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D292">
@@ -13968,10 +14966,16 @@
       <c r="J292">
         <v>0.3794304793144223</v>
       </c>
+      <c r="K292">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L292">
         <v>24917</v>
       </c>
       <c r="M292">
+        <v>55570</v>
+      </c>
+      <c r="N292">
         <v>34.39</v>
       </c>
     </row>
@@ -13988,7 +14992,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D293">
@@ -14012,10 +15016,16 @@
       <c r="J293">
         <v>5.542966561887937</v>
       </c>
+      <c r="K293">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L293">
         <v>0</v>
       </c>
       <c r="M293">
+        <v>56450</v>
+      </c>
+      <c r="N293">
         <v>33.68</v>
       </c>
     </row>
@@ -14032,7 +15042,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D294">
@@ -14056,10 +15066,16 @@
       <c r="J294">
         <v>2.213948002214585</v>
       </c>
+      <c r="K294">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L294">
         <v>0</v>
       </c>
       <c r="M294">
+        <v>61200</v>
+      </c>
+      <c r="N294">
         <v>11.93</v>
       </c>
     </row>
@@ -14076,7 +15092,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D295">
@@ -14100,10 +15116,16 @@
       <c r="J295">
         <v>0.1853509962461325</v>
       </c>
+      <c r="K295">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L295">
         <v>0</v>
       </c>
       <c r="M295">
+        <v>53460</v>
+      </c>
+      <c r="N295">
         <v>67.91</v>
       </c>
     </row>
@@ -14120,7 +15142,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D296">
@@ -14144,10 +15166,16 @@
       <c r="J296">
         <v>36.32222499731586</v>
       </c>
+      <c r="K296">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L296">
         <v>12411</v>
       </c>
       <c r="M296">
+        <v>55470</v>
+      </c>
+      <c r="N296">
         <v>100</v>
       </c>
     </row>
@@ -14164,7 +15192,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D297">
@@ -14188,10 +15216,16 @@
       <c r="J297">
         <v>41.39691448249086</v>
       </c>
+      <c r="K297">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L297">
         <v>0</v>
       </c>
       <c r="M297">
+        <v>51080</v>
+      </c>
+      <c r="N297">
         <v>57.33</v>
       </c>
     </row>
@@ -14208,7 +15242,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D298">
@@ -14232,10 +15266,16 @@
       <c r="J298">
         <v>0.3115826552877649</v>
       </c>
+      <c r="K298">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L298">
         <v>269923</v>
       </c>
       <c r="M298">
+        <v>57150</v>
+      </c>
+      <c r="N298">
         <v>27.01</v>
       </c>
     </row>
@@ -14252,7 +15292,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D299">
@@ -14276,10 +15316,16 @@
       <c r="J299">
         <v>0.1071880455514616</v>
       </c>
+      <c r="K299">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L299">
         <v>78552</v>
       </c>
       <c r="M299">
+        <v>51120</v>
+      </c>
+      <c r="N299">
         <v>99.84999999999999</v>
       </c>
     </row>
@@ -14296,7 +15342,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D300">
@@ -14320,10 +15366,16 @@
       <c r="J300">
         <v>0.3860790644001836</v>
       </c>
+      <c r="K300">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L300">
         <v>0</v>
       </c>
       <c r="M300">
+        <v>55620</v>
+      </c>
+      <c r="N300">
         <v>31.9</v>
       </c>
     </row>
@@ -14340,7 +15392,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D301">
@@ -14364,10 +15416,16 @@
       <c r="J301">
         <v>0.3610894756160769</v>
       </c>
+      <c r="K301">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L301">
         <v>47166</v>
       </c>
       <c r="M301">
+        <v>53770</v>
+      </c>
+      <c r="N301">
         <v>29.89</v>
       </c>
     </row>
@@ -14384,7 +15442,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D302">
@@ -14408,10 +15466,16 @@
       <c r="J302">
         <v>24.54082546958647</v>
       </c>
+      <c r="K302">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L302">
         <v>0</v>
       </c>
       <c r="M302">
+        <v>51840</v>
+      </c>
+      <c r="N302">
         <v>68.87</v>
       </c>
     </row>
@@ -14428,7 +15492,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D303">
@@ -14452,10 +15516,16 @@
       <c r="J303">
         <v>61.31517863667393</v>
       </c>
+      <c r="K303">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L303">
         <v>2280</v>
       </c>
       <c r="M303">
+        <v>51970</v>
+      </c>
+      <c r="N303">
         <v>83.09</v>
       </c>
     </row>
@@ -14472,7 +15542,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D304">
@@ -14496,10 +15566,16 @@
       <c r="J304">
         <v>75.67484654329289</v>
       </c>
+      <c r="K304">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L304">
         <v>0</v>
       </c>
       <c r="M304">
+        <v>52170</v>
+      </c>
+      <c r="N304">
         <v>47.75</v>
       </c>
     </row>
@@ -14516,7 +15592,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D305">
@@ -14540,10 +15616,16 @@
       <c r="J305">
         <v>65.2200782971381</v>
       </c>
+      <c r="K305">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L305">
         <v>14363</v>
       </c>
       <c r="M305">
+        <v>51960</v>
+      </c>
+      <c r="N305">
         <v>72.72</v>
       </c>
     </row>
@@ -14560,7 +15642,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D306">
@@ -14584,10 +15666,16 @@
       <c r="J306">
         <v>0.18229686884876</v>
       </c>
+      <c r="K306">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L306">
         <v>21962</v>
       </c>
       <c r="M306">
+        <v>52880</v>
+      </c>
+      <c r="N306">
         <v>53.06</v>
       </c>
     </row>
@@ -14604,7 +15692,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D307">
@@ -14628,10 +15716,16 @@
       <c r="J307">
         <v>18.165499124931</v>
       </c>
+      <c r="K307">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L307">
         <v>0</v>
       </c>
       <c r="M307">
+        <v>52770</v>
+      </c>
+      <c r="N307">
         <v>69.72</v>
       </c>
     </row>
@@ -14648,7 +15742,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D308">
@@ -14672,10 +15766,16 @@
       <c r="J308">
         <v>17.90832820202273</v>
       </c>
+      <c r="K308">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L308">
         <v>3064</v>
       </c>
       <c r="M308">
+        <v>54190</v>
+      </c>
+      <c r="N308">
         <v>50.2</v>
       </c>
     </row>
@@ -14692,7 +15792,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D309">
@@ -14716,10 +15816,16 @@
       <c r="J309">
         <v>28.83796633385532</v>
       </c>
+      <c r="K309">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L309">
         <v>12440</v>
       </c>
       <c r="M309">
+        <v>53610</v>
+      </c>
+      <c r="N309">
         <v>52.51</v>
       </c>
     </row>
@@ -14736,7 +15842,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D310">
@@ -14760,10 +15866,16 @@
       <c r="J310">
         <v>25.71915897389005</v>
       </c>
+      <c r="K310">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L310">
         <v>14480</v>
       </c>
       <c r="M310">
+        <v>53550</v>
+      </c>
+      <c r="N310">
         <v>99.5</v>
       </c>
     </row>
@@ -14780,7 +15892,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D311">
@@ -14804,10 +15916,16 @@
       <c r="J311">
         <v>0.5078991917759708</v>
       </c>
+      <c r="K311">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L311">
         <v>0</v>
       </c>
       <c r="M311">
+        <v>54800</v>
+      </c>
+      <c r="N311">
         <v>53.57</v>
       </c>
     </row>
@@ -14824,7 +15942,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D312">
@@ -14848,10 +15966,16 @@
       <c r="J312">
         <v>0.1713157195221743</v>
       </c>
+      <c r="K312">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L312">
         <v>0</v>
       </c>
       <c r="M312">
+        <v>52970</v>
+      </c>
+      <c r="N312">
         <v>60.74</v>
       </c>
     </row>
@@ -14868,7 +15992,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D313">
@@ -14892,10 +16016,16 @@
       <c r="J313">
         <v>0.001737111854873408</v>
       </c>
+      <c r="K313">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L313">
         <v>20967</v>
       </c>
       <c r="M313">
+        <v>55360</v>
+      </c>
+      <c r="N313">
         <v>53.93</v>
       </c>
     </row>
@@ -14912,7 +16042,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D314">
@@ -14936,10 +16066,16 @@
       <c r="J314">
         <v>0.1511213078816971</v>
       </c>
+      <c r="K314">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L314">
         <v>77464</v>
       </c>
       <c r="M314">
+        <v>53940</v>
+      </c>
+      <c r="N314">
         <v>64.72</v>
       </c>
     </row>
@@ -14956,7 +16092,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D315">
@@ -14980,10 +16116,16 @@
       <c r="J315">
         <v>0.1222331099894117</v>
       </c>
+      <c r="K315">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L315">
         <v>20814</v>
       </c>
       <c r="M315">
+        <v>56410</v>
+      </c>
+      <c r="N315">
         <v>47.68</v>
       </c>
     </row>
@@ -15000,7 +16142,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D316">
@@ -15024,10 +16166,16 @@
       <c r="J316">
         <v>0.1662148061744048</v>
       </c>
+      <c r="K316">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L316">
         <v>34196</v>
       </c>
       <c r="M316">
+        <v>53690</v>
+      </c>
+      <c r="N316">
         <v>68.03</v>
       </c>
     </row>
@@ -15044,7 +16192,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>SØR-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D317">
@@ -15068,10 +16216,16 @@
       <c r="J317">
         <v>0.290013456336721</v>
       </c>
+      <c r="K317">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L317">
         <v>43884</v>
       </c>
       <c r="M317">
+        <v>53810</v>
+      </c>
+      <c r="N317">
         <v>35.41</v>
       </c>
     </row>
@@ -15088,7 +16242,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>NORD-TRØNDELAG</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D318">
@@ -15112,10 +16266,16 @@
       <c r="J318">
         <v>0.1672469212363001</v>
       </c>
+      <c r="K318">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L318">
         <v>16210</v>
       </c>
       <c r="M318">
+        <v>55510</v>
+      </c>
+      <c r="N318">
         <v>41.84</v>
       </c>
     </row>
@@ -15132,7 +16292,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>TrC8ndelag</t>
+          <t>Trøndelag</t>
         </is>
       </c>
       <c r="D319">
@@ -15156,10 +16316,16 @@
       <c r="J319">
         <v>26.01845859168469</v>
       </c>
+      <c r="K319">
+        <v>58.06874999999999</v>
+      </c>
       <c r="L319">
         <v>0</v>
       </c>
       <c r="M319">
+        <v>52170</v>
+      </c>
+      <c r="N319">
         <v>62.92</v>
       </c>
     </row>
@@ -15207,6 +16373,9 @@
         <v>1184871</v>
       </c>
       <c r="M320">
+        <v>58230</v>
+      </c>
+      <c r="N320">
         <v>8.779999999999999</v>
       </c>
     </row>
@@ -15254,6 +16423,9 @@
         <v>174436</v>
       </c>
       <c r="M321">
+        <v>57230</v>
+      </c>
+      <c r="N321">
         <v>14.28</v>
       </c>
     </row>
@@ -15301,6 +16473,9 @@
         <v>0</v>
       </c>
       <c r="M322">
+        <v>53710</v>
+      </c>
+      <c r="N322">
         <v>37.29</v>
       </c>
     </row>
@@ -15348,6 +16523,9 @@
         <v>0</v>
       </c>
       <c r="M323">
+        <v>55050</v>
+      </c>
+      <c r="N323">
         <v>61.46</v>
       </c>
     </row>
@@ -15395,6 +16573,9 @@
         <v>0</v>
       </c>
       <c r="M324">
+        <v>54030</v>
+      </c>
+      <c r="N324">
         <v>64.68000000000001</v>
       </c>
     </row>
@@ -15442,6 +16623,9 @@
         <v>0</v>
       </c>
       <c r="M325">
+        <v>50900</v>
+      </c>
+      <c r="N325">
         <v>100</v>
       </c>
     </row>
@@ -15489,6 +16673,9 @@
         <v>10128</v>
       </c>
       <c r="M326">
+        <v>51250</v>
+      </c>
+      <c r="N326">
         <v>69.56999999999999</v>
       </c>
     </row>
@@ -15536,6 +16723,9 @@
         <v>7826</v>
       </c>
       <c r="M327">
+        <v>56320</v>
+      </c>
+      <c r="N327">
         <v>36.25</v>
       </c>
     </row>
@@ -15583,6 +16773,9 @@
         <v>0</v>
       </c>
       <c r="M328">
+        <v>53810</v>
+      </c>
+      <c r="N328">
         <v>61.58</v>
       </c>
     </row>
@@ -15630,6 +16823,9 @@
         <v>16898</v>
       </c>
       <c r="M329">
+        <v>54860</v>
+      </c>
+      <c r="N329">
         <v>42.51</v>
       </c>
     </row>
@@ -15677,6 +16873,9 @@
         <v>10923</v>
       </c>
       <c r="M330">
+        <v>54200</v>
+      </c>
+      <c r="N330">
         <v>44.13</v>
       </c>
     </row>
@@ -15724,6 +16923,9 @@
         <v>8315</v>
       </c>
       <c r="M331">
+        <v>52450</v>
+      </c>
+      <c r="N331">
         <v>100</v>
       </c>
     </row>
@@ -15771,6 +16973,9 @@
         <v>154744</v>
       </c>
       <c r="M332">
+        <v>53670</v>
+      </c>
+      <c r="N332">
         <v>45.88</v>
       </c>
     </row>
@@ -15818,6 +17023,9 @@
         <v>0</v>
       </c>
       <c r="M333">
+        <v>52580</v>
+      </c>
+      <c r="N333">
         <v>70.56</v>
       </c>
     </row>
@@ -15865,6 +17073,9 @@
         <v>14714</v>
       </c>
       <c r="M334">
+        <v>50870</v>
+      </c>
+      <c r="N334">
         <v>76.75</v>
       </c>
     </row>
@@ -15912,6 +17123,9 @@
         <v>18449</v>
       </c>
       <c r="M335">
+        <v>52340</v>
+      </c>
+      <c r="N335">
         <v>63.62</v>
       </c>
     </row>
@@ -15959,6 +17173,9 @@
         <v>60955</v>
       </c>
       <c r="M336">
+        <v>51460</v>
+      </c>
+      <c r="N336">
         <v>70.41</v>
       </c>
     </row>
@@ -16006,6 +17223,9 @@
         <v>0</v>
       </c>
       <c r="M337">
+        <v>53390</v>
+      </c>
+      <c r="N337">
         <v>72.95</v>
       </c>
     </row>
@@ -16053,6 +17273,9 @@
         <v>18994</v>
       </c>
       <c r="M338">
+        <v>52640</v>
+      </c>
+      <c r="N338">
         <v>12.03</v>
       </c>
     </row>
@@ -16100,6 +17323,9 @@
         <v>10439</v>
       </c>
       <c r="M339">
+        <v>53880</v>
+      </c>
+      <c r="N339">
         <v>42.8</v>
       </c>
     </row>
@@ -16147,6 +17373,9 @@
         <v>12189</v>
       </c>
       <c r="M340">
+        <v>53350</v>
+      </c>
+      <c r="N340">
         <v>64.13</v>
       </c>
     </row>
@@ -16194,6 +17423,9 @@
         <v>223353</v>
       </c>
       <c r="M341">
+        <v>55570</v>
+      </c>
+      <c r="N341">
         <v>17.38</v>
       </c>
     </row>
@@ -16241,6 +17473,9 @@
         <v>109594</v>
       </c>
       <c r="M342">
+        <v>57600</v>
+      </c>
+      <c r="N342">
         <v>10.78</v>
       </c>
     </row>
@@ -16288,6 +17523,9 @@
         <v>11341</v>
       </c>
       <c r="M343">
+        <v>55160</v>
+      </c>
+      <c r="N343">
         <v>19.84</v>
       </c>
     </row>
@@ -16335,6 +17573,9 @@
         <v>11696</v>
       </c>
       <c r="M344">
+        <v>55640</v>
+      </c>
+      <c r="N344">
         <v>7.78</v>
       </c>
     </row>
@@ -16382,6 +17623,9 @@
         <v>0</v>
       </c>
       <c r="M345">
+        <v>53120</v>
+      </c>
+      <c r="N345">
         <v>29.63</v>
       </c>
     </row>
@@ -16429,6 +17673,9 @@
         <v>0</v>
       </c>
       <c r="M346">
+        <v>52500</v>
+      </c>
+      <c r="N346">
         <v>47.75</v>
       </c>
     </row>
@@ -16476,6 +17723,9 @@
         <v>18604</v>
       </c>
       <c r="M347">
+        <v>50540</v>
+      </c>
+      <c r="N347">
         <v>43.29</v>
       </c>
     </row>
@@ -16523,6 +17773,9 @@
         <v>0</v>
       </c>
       <c r="M348">
+        <v>49500</v>
+      </c>
+      <c r="N348">
         <v>31.56</v>
       </c>
     </row>
@@ -16570,6 +17823,9 @@
         <v>0</v>
       </c>
       <c r="M349">
+        <v>50620</v>
+      </c>
+      <c r="N349">
         <v>17.43</v>
       </c>
     </row>
@@ -16617,6 +17873,9 @@
         <v>107475</v>
       </c>
       <c r="M350">
+        <v>52840</v>
+      </c>
+      <c r="N350">
         <v>9.93</v>
       </c>
     </row>
@@ -16664,6 +17923,9 @@
         <v>32815</v>
       </c>
       <c r="M351">
+        <v>54400</v>
+      </c>
+      <c r="N351">
         <v>42.07</v>
       </c>
     </row>
@@ -16711,6 +17973,9 @@
         <v>0</v>
       </c>
       <c r="M352">
+        <v>52140</v>
+      </c>
+      <c r="N352">
         <v>30.86</v>
       </c>
     </row>
@@ -16758,6 +18023,9 @@
         <v>0</v>
       </c>
       <c r="M353">
+        <v>49620</v>
+      </c>
+      <c r="N353">
         <v>12.34</v>
       </c>
     </row>
@@ -16805,6 +18073,9 @@
         <v>5990</v>
       </c>
       <c r="M354">
+        <v>52700</v>
+      </c>
+      <c r="N354">
         <v>73.34999999999999</v>
       </c>
     </row>
@@ -16852,6 +18123,9 @@
         <v>0</v>
       </c>
       <c r="M355">
+        <v>50840</v>
+      </c>
+      <c r="N355">
         <v>3.7</v>
       </c>
     </row>
@@ -16899,6 +18173,9 @@
         <v>0</v>
       </c>
       <c r="M356">
+        <v>49730</v>
+      </c>
+      <c r="N356">
         <v>0.14</v>
       </c>
     </row>
@@ -16946,6 +18223,9 @@
         <v>0</v>
       </c>
       <c r="M357">
+        <v>52250</v>
+      </c>
+      <c r="N357">
         <v>10.09</v>
       </c>
     </row>
@@ -16993,6 +18273,9 @@
         <v>0</v>
       </c>
       <c r="M358">
+        <v>52820</v>
+      </c>
+      <c r="N358">
         <v>100</v>
       </c>
     </row>

</xml_diff>